<commit_message>
Suite Analyse et début code Inscription et connexion
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>Activités</t>
   </si>
@@ -225,6 +225,69 @@
   </si>
   <si>
     <t>10.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Suite de mon analyse en continuant les différents points de mon analyse.</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Documentation</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, BDD</t>
+  </si>
+  <si>
+    <t>Création du script de la base de donnée grâce au MLD sur Workbench</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Code</t>
+  </si>
+  <si>
+    <t>Mise en place de l'environnement afin de coder mon site Task&amp;Go</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Code vue Accueil</t>
+  </si>
+  <si>
+    <t>Création de la vue de mon Accueil comme spécifié dans mon cahier des charges</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Code vue Inscription</t>
+  </si>
+  <si>
+    <t>Création du MVC à partir de 0, création de mon propre template pour ce projet</t>
+  </si>
+  <si>
+    <t>Création de la vue Inscription</t>
+  </si>
+  <si>
+    <t>Diego Sanchez et Kevin Pasteur, MCD</t>
+  </si>
+  <si>
+    <t>Correction de son MCD et de ses différentes cardinalitées</t>
+  </si>
+  <si>
+    <t>Création du fonctionnement de l'inscription, sans test ni vérification de donnée</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Code vue Connexion</t>
+  </si>
+  <si>
+    <t>Création de la page vue connexion ainsi que le bon focntionnement de la connexion d'un utilisateur de la base de donnée</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Test intégration</t>
+  </si>
+  <si>
+    <t>Teste de l'inscription suivit de la connexion avec ce compte, et réglage des quelques petits problèmes rencontrés durant ma phase de test</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Mise en ligne</t>
+  </si>
+  <si>
+    <t>Prise en main de SwissCenter afin de pouvoir mettre mon début de code en ligne est de l'accéder depuis différents appareils, site pas encore en ligne !</t>
+  </si>
+  <si>
+    <t>Début du code et finalisation de l'analyse, je suis plutôt content de la vitesse où j'avance.</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1747,30 +1810,415 @@
       <c r="H39" s="24"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="24"/>
+      <c r="C40" s="50">
+        <v>43599</v>
+      </c>
+      <c r="D40" s="30">
+        <v>30</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="23"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="8"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="30">
+        <v>15</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" s="45"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="30">
+        <v>45</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="45"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="30">
+        <v>45</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43" s="45"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="30">
+        <v>45</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="45"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="30">
+        <v>45</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="45"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="30">
+        <v>45</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="45"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="30">
+        <v>45</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="45"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="30">
+        <v>15</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="45"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="4"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="30">
+        <v>30</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="45"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="4"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="30">
+        <v>45</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" s="46"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="4"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="30">
+        <f>SUM(D40:D50)</f>
+        <v>405</v>
+      </c>
+      <c r="E51" s="25"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="4"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="4"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="4"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="4"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="4"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="4"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="4"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="4"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="4"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="4"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="4"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="4"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="4"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="4"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="4"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="8"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="9"/>
+    </row>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A1:E2"/>

</xml_diff>

<commit_message>
Inscription et Connexion fonctionnelle + Suite de l'analyse
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Activités</t>
   </si>
@@ -288,13 +288,43 @@
   </si>
   <si>
     <t>Début du code et finalisation de l'analyse, je suis plutôt content de la vitesse où j'avance.</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Inscription</t>
+  </si>
+  <si>
+    <t>Finalisation de mon inscription au site avec toutes les différentes vérifications des champs et des données entré par le visiteur. Inscription de la base de donnée</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Connexion</t>
+  </si>
+  <si>
+    <t>Finalisation de ma connexion au site, vérification des champs et des données entré par le visiteur</t>
+  </si>
+  <si>
+    <t>Teste de l'inscription suivit de la connexion avec ce compte, ces tests sont réalisé en testant tous les champs et leurs vérifications</t>
+  </si>
+  <si>
+    <t>14.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Suite de mon analyse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de différents compte et accèes en vue de mettre mon site en ligne, actuellement pas en ligne </t>
+  </si>
+  <si>
+    <t>15.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Mise en place de mon inscription et de ma connexion au site. La mise en ligne me pose quelques problèmes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -328,8 +358,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +384,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -602,11 +644,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -717,6 +760,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -726,29 +778,30 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -1197,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1218,31 +1271,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="51"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1304,7 +1357,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="47">
+      <c r="C9" s="53">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1316,7 +1369,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="52" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1324,7 +1377,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="48"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="30">
         <v>75</v>
       </c>
@@ -1334,13 +1387,13 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="45"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="48"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="30">
         <v>45</v>
       </c>
@@ -1350,13 +1403,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="45"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="48"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="30">
         <v>75</v>
       </c>
@@ -1366,13 +1419,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="48"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="30">
         <v>15</v>
       </c>
@@ -1382,13 +1435,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="45"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="48"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="30">
         <v>30</v>
       </c>
@@ -1398,13 +1451,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="48"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="48"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="30">
         <v>75</v>
       </c>
@@ -1414,13 +1467,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="45"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="49"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="30">
         <v>30</v>
       </c>
@@ -1430,7 +1483,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="46"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1451,7 +1504,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="50">
+      <c r="C18" s="44">
         <v>43593</v>
       </c>
       <c r="D18" s="30">
@@ -1463,7 +1516,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="47" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1471,7 +1524,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="48"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="30">
         <v>90</v>
       </c>
@@ -1481,13 +1534,13 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="49"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="30">
         <v>45</v>
       </c>
@@ -1497,7 +1550,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="46"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1518,7 +1571,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="50">
+      <c r="C22" s="44">
         <v>43594</v>
       </c>
       <c r="D22" s="30">
@@ -1530,7 +1583,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="47" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1538,7 +1591,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="48"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="30">
         <v>30</v>
       </c>
@@ -1548,13 +1601,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="48"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="30">
         <v>70</v>
       </c>
@@ -1564,13 +1617,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="45"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="48"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="30">
         <v>35</v>
       </c>
@@ -1580,13 +1633,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="45"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="48"/>
+      <c r="C26" s="45"/>
       <c r="D26" s="30">
         <v>20</v>
       </c>
@@ -1596,13 +1649,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="45"/>
+      <c r="G26" s="48"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="48"/>
+      <c r="C27" s="45"/>
       <c r="D27" s="30">
         <v>45</v>
       </c>
@@ -1612,13 +1665,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="45"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="48"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="30">
         <v>55</v>
       </c>
@@ -1628,13 +1681,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="45"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="48"/>
+      <c r="C29" s="45"/>
       <c r="D29" s="30">
         <v>70</v>
       </c>
@@ -1644,13 +1697,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="45"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="49"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="30">
         <v>20</v>
       </c>
@@ -1660,7 +1713,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="46"/>
+      <c r="G30" s="49"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1681,7 +1734,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="50">
+      <c r="C32" s="44">
         <v>43595</v>
       </c>
       <c r="D32" s="30">
@@ -1693,7 +1746,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="44" t="s">
+      <c r="G32" s="47" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1701,7 +1754,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="48"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="30">
         <v>45</v>
       </c>
@@ -1711,13 +1764,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="45"/>
+      <c r="G33" s="48"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="48"/>
+      <c r="C34" s="45"/>
       <c r="D34" s="30">
         <v>70</v>
       </c>
@@ -1727,13 +1780,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="45"/>
+      <c r="G34" s="48"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="48"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="30">
         <v>90</v>
       </c>
@@ -1743,13 +1796,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="45"/>
+      <c r="G35" s="48"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="48"/>
+      <c r="C36" s="45"/>
       <c r="D36" s="30">
         <v>45</v>
       </c>
@@ -1759,13 +1812,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="45"/>
+      <c r="G36" s="48"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="48"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="30">
         <v>20</v>
       </c>
@@ -1775,13 +1828,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="45"/>
+      <c r="G37" s="48"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="49"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="30">
         <v>25</v>
       </c>
@@ -1791,7 +1844,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="46"/>
+      <c r="G38" s="49"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -1812,7 +1865,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="50">
+      <c r="C40" s="44">
         <v>43599</v>
       </c>
       <c r="D40" s="30">
@@ -1824,7 +1877,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="44" t="s">
+      <c r="G40" s="47" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -1832,7 +1885,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="48"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="30">
         <v>15</v>
       </c>
@@ -1842,13 +1895,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="45"/>
+      <c r="G41" s="48"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="48"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="30">
         <v>45</v>
       </c>
@@ -1858,13 +1911,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="45"/>
+      <c r="G42" s="48"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="48"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="30">
         <v>45</v>
       </c>
@@ -1874,13 +1927,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="45"/>
+      <c r="G43" s="48"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="48"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="30">
         <v>45</v>
       </c>
@@ -1890,13 +1943,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="45"/>
+      <c r="G44" s="48"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="48"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="30">
         <v>45</v>
       </c>
@@ -1906,13 +1959,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="45"/>
+      <c r="G45" s="48"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="48"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="30">
         <v>45</v>
       </c>
@@ -1922,13 +1975,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="45"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="48"/>
+      <c r="C47" s="45"/>
       <c r="D47" s="30">
         <v>45</v>
       </c>
@@ -1938,13 +1991,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="45"/>
+      <c r="G47" s="48"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="48"/>
+      <c r="C48" s="45"/>
       <c r="D48" s="30">
         <v>15</v>
       </c>
@@ -1954,13 +2007,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="45"/>
+      <c r="G48" s="48"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="48"/>
+      <c r="C49" s="45"/>
       <c r="D49" s="30">
         <v>30</v>
       </c>
@@ -1970,13 +2023,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="45"/>
+      <c r="G49" s="48"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="49"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="30">
         <v>45</v>
       </c>
@@ -1986,13 +2039,15 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="46"/>
+      <c r="G50" s="49"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="4"/>
-      <c r="C51" s="20"/>
+      <c r="C51" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="D51" s="30">
         <f>SUM(D40:D50)</f>
         <v>405</v>
@@ -2003,60 +2058,99 @@
       <c r="H51" s="24"/>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="24"/>
+      <c r="C52" s="44">
+        <v>43600</v>
+      </c>
+      <c r="D52" s="30">
+        <v>60</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" s="23"/>
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="24"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="30">
+        <v>60</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53" s="55"/>
+      <c r="H53" s="23"/>
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="24"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="30">
+        <v>45</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="55"/>
+      <c r="H54" s="23"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="24"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="30">
+        <v>15</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G55" s="55"/>
+      <c r="H55" s="23"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="24"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="30">
+        <v>45</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G56" s="56"/>
+      <c r="H56" s="23"/>
       <c r="I56" s="5"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="30"/>
+      <c r="C57" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="30">
+        <f>SUM(D52:D56)</f>
+        <v>225</v>
+      </c>
       <c r="E57" s="25"/>
       <c r="F57" s="14"/>
       <c r="G57" s="30"/>
@@ -2084,143 +2178,19 @@
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="4"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B61" s="4"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B62" s="4"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="4"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="24"/>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B64" s="4"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B65" s="4"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="24"/>
-      <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B66" s="4"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B67" s="4"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B68" s="4"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B69" s="4"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B70" s="4"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="5"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B71" s="4"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B72" s="8"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="9"/>
-    </row>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
+  <mergeCells count="15">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -2230,6 +2200,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Création de la vue calendrier + suite de la vérification des données dans les champs
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
   <si>
     <t>Activités</t>
   </si>
@@ -318,6 +318,48 @@
   </si>
   <si>
     <t>Mise en place de mon inscription et de ma connexion au site. La mise en ligne me pose quelques problèmes.</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Planification détaillé</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Théorie ICT-431</t>
+  </si>
+  <si>
+    <t>Création de ma planification à partir de ma planification initiale, dévellopement de mes tâches en profondeur afin d'eclaircire ma planification</t>
+  </si>
+  <si>
+    <t>Relecture de la théorie du module ICT- 431 sur la stratégie de test et la réalisation des tests à faire.</t>
+  </si>
+  <si>
+    <t>Suite et correction de mon analyse en relisant quelques points de mon rapport de projet</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Correction code</t>
+  </si>
+  <si>
+    <t>Correction de passablement de points qui n'était pas encore ajouter à mon inscription ainsi qu'à ma connexion (champs, vérification de droit)</t>
+  </si>
+  <si>
+    <t>Création du header afin d'ajouter mon menu dans le header dépendant de la permission de l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Rechercher du problème de ma mise en ligne de hier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en ligne de mon site, et création de la base de donnée en ligne </t>
+  </si>
+  <si>
+    <t>Cryptage du mot de passe dans la bdd pour l'inscription et la connexion, cryptage en SHA1</t>
+  </si>
+  <si>
+    <t>Création de la vue affichage d'un calendrier, affichage d'un calendrier basique et modification de celui-ci.</t>
+  </si>
+  <si>
+    <t>16.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Mise en ligne du site, ainsi que modification des modules déjà mit en place sur le site.</t>
   </si>
 </sst>
 </file>
@@ -390,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -643,13 +685,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -760,36 +822,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -798,6 +860,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1250,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1271,31 +1351,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1357,7 +1437,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="53">
+      <c r="C9" s="49">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1369,7 +1449,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="45" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1377,7 +1457,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="45"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="30">
         <v>75</v>
       </c>
@@ -1387,13 +1467,13 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="48"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="45"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="30">
         <v>45</v>
       </c>
@@ -1403,13 +1483,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="48"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="45"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="30">
         <v>75</v>
       </c>
@@ -1419,13 +1499,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="48"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="45"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="30">
         <v>15</v>
       </c>
@@ -1435,13 +1515,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="48"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="30">
         <v>30</v>
       </c>
@@ -1451,13 +1531,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="48"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="30">
         <v>75</v>
       </c>
@@ -1467,13 +1547,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="48"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="46"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="30">
         <v>30</v>
       </c>
@@ -1483,7 +1563,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="49"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1504,7 +1584,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="44">
+      <c r="C18" s="52">
         <v>43593</v>
       </c>
       <c r="D18" s="30">
@@ -1516,7 +1596,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="48" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1524,7 +1604,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="45"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="30">
         <v>90</v>
       </c>
@@ -1534,13 +1614,13 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="48"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="46"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="30">
         <v>45</v>
       </c>
@@ -1550,7 +1630,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="49"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1571,7 +1651,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="44">
+      <c r="C22" s="52">
         <v>43594</v>
       </c>
       <c r="D22" s="30">
@@ -1583,7 +1663,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="48" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1591,7 +1671,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="30">
         <v>30</v>
       </c>
@@ -1601,13 +1681,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="46"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="30">
         <v>70</v>
       </c>
@@ -1617,13 +1697,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="48"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="30">
         <v>35</v>
       </c>
@@ -1633,13 +1713,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="48"/>
+      <c r="G25" s="46"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="45"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="30">
         <v>20</v>
       </c>
@@ -1649,13 +1729,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="48"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="45"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="30">
         <v>45</v>
       </c>
@@ -1665,13 +1745,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="48"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="45"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="30">
         <v>55</v>
       </c>
@@ -1681,13 +1761,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="48"/>
+      <c r="G28" s="46"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="45"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="30">
         <v>70</v>
       </c>
@@ -1697,13 +1777,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="48"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="46"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="30">
         <v>20</v>
       </c>
@@ -1713,7 +1793,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="49"/>
+      <c r="G30" s="47"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1734,7 +1814,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="44">
+      <c r="C32" s="52">
         <v>43595</v>
       </c>
       <c r="D32" s="30">
@@ -1746,7 +1826,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="47" t="s">
+      <c r="G32" s="48" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1754,7 +1834,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="45"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="30">
         <v>45</v>
       </c>
@@ -1764,13 +1844,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="48"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="45"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="30">
         <v>70</v>
       </c>
@@ -1780,13 +1860,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="48"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="45"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="30">
         <v>90</v>
       </c>
@@ -1796,13 +1876,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="48"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="45"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="30">
         <v>45</v>
       </c>
@@ -1812,13 +1892,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="48"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="45"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="30">
         <v>20</v>
       </c>
@@ -1828,13 +1908,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="48"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="46"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="30">
         <v>25</v>
       </c>
@@ -1844,7 +1924,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="49"/>
+      <c r="G38" s="47"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -1865,7 +1945,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="44">
+      <c r="C40" s="52">
         <v>43599</v>
       </c>
       <c r="D40" s="30">
@@ -1877,7 +1957,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="G40" s="48" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -1885,7 +1965,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="45"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="30">
         <v>15</v>
       </c>
@@ -1895,13 +1975,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="48"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="45"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="30">
         <v>45</v>
       </c>
@@ -1911,13 +1991,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="48"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="45"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="30">
         <v>45</v>
       </c>
@@ -1927,13 +2007,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="48"/>
+      <c r="G43" s="46"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="45"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="30">
         <v>45</v>
       </c>
@@ -1943,13 +2023,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="48"/>
+      <c r="G44" s="46"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="45"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="30">
         <v>45</v>
       </c>
@@ -1959,13 +2039,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="48"/>
+      <c r="G45" s="46"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="45"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="30">
         <v>45</v>
       </c>
@@ -1975,13 +2055,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="48"/>
+      <c r="G46" s="46"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="45"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="30">
         <v>45</v>
       </c>
@@ -1991,13 +2071,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="48"/>
+      <c r="G47" s="46"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="45"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="30">
         <v>15</v>
       </c>
@@ -2007,13 +2087,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="48"/>
+      <c r="G48" s="46"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="45"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="30">
         <v>30</v>
       </c>
@@ -2023,13 +2103,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="48"/>
+      <c r="G49" s="46"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="46"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="30">
         <v>45</v>
       </c>
@@ -2039,7 +2119,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="49"/>
+      <c r="G50" s="47"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
@@ -2060,7 +2140,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="44">
+      <c r="C52" s="52">
         <v>43600</v>
       </c>
       <c r="D52" s="30">
@@ -2080,7 +2160,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="45"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="30">
         <v>60</v>
       </c>
@@ -2096,7 +2176,7 @@
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="45"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="30">
         <v>45</v>
       </c>
@@ -2112,7 +2192,7 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="45"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="30">
         <v>15</v>
       </c>
@@ -2128,7 +2208,7 @@
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="46"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="30">
         <v>45</v>
       </c>
@@ -2157,40 +2237,291 @@
       <c r="H57" s="24"/>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="24"/>
+      <c r="C58" s="52">
+        <v>43601</v>
+      </c>
+      <c r="D58" s="30">
+        <v>30</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G58" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="H58" s="23"/>
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="24"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="30">
+        <v>15</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G59" s="46"/>
+      <c r="H59" s="23"/>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="8"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="9"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="30">
+        <v>45</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60" s="46"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="4"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="30">
+        <v>90</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G61" s="46"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B62" s="4"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="58">
+        <v>30</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" s="46"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="4"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="30">
+        <v>15</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G63" s="46"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B64" s="4"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="30">
+        <v>45</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="46"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B65" s="4"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="30">
+        <v>45</v>
+      </c>
+      <c r="E65" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G65" s="46"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B66" s="4"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="30">
+        <v>90</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" s="47"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="4"/>
+      <c r="C67" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="58">
+        <f>SUM(D58:D66)</f>
+        <v>405</v>
+      </c>
+      <c r="E67" s="59"/>
+      <c r="F67" s="60"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="61"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="4"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="4"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="4"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="4"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="4"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="4"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="4"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="4"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="4"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="4"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="58"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="60"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="61"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B78" s="8"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -2200,12 +2531,6 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Suite du code + fin analyse
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>Activités</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>Mise en ligne du site, ainsi que modification des modules déjà mit en place sur le site.</t>
+  </si>
+  <si>
+    <t>Création de la vue Mes tâches et rendez-vous et quelques retouches sur le calendrier de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, fin Analyse</t>
+  </si>
+  <si>
+    <t>Relecture de ma planification détaillée + insertion de celle-ci dans mon rapport de projet et relecture de toute mon analyse</t>
   </si>
 </sst>
 </file>
@@ -822,62 +831,62 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1330,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1351,31 +1360,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="53"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1437,7 +1446,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="49">
+      <c r="C9" s="62">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1449,7 +1458,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="61" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1457,7 +1466,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="30">
         <v>75</v>
       </c>
@@ -1467,13 +1476,13 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="46"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="30">
         <v>45</v>
       </c>
@@ -1483,13 +1492,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="46"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="30">
         <v>75</v>
       </c>
@@ -1499,13 +1508,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="46"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="30">
         <v>15</v>
       </c>
@@ -1515,13 +1524,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="46"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="30">
         <v>30</v>
       </c>
@@ -1531,13 +1540,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="46"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="30">
         <v>75</v>
       </c>
@@ -1547,13 +1556,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="46"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="30">
         <v>30</v>
       </c>
@@ -1563,7 +1572,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="47"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1584,7 +1593,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="52">
+      <c r="C18" s="50">
         <v>43593</v>
       </c>
       <c r="D18" s="30">
@@ -1596,7 +1605,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="53" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1604,7 +1613,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="30">
         <v>90</v>
       </c>
@@ -1614,13 +1623,13 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="46"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="51"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="30">
         <v>45</v>
       </c>
@@ -1630,7 +1639,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="47"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1651,7 +1660,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="52">
+      <c r="C22" s="50">
         <v>43594</v>
       </c>
       <c r="D22" s="30">
@@ -1663,7 +1672,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="53" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1671,7 +1680,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="50"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="30">
         <v>30</v>
       </c>
@@ -1681,13 +1690,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="46"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="50"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="30">
         <v>70</v>
       </c>
@@ -1697,13 +1706,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="46"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="30">
         <v>35</v>
       </c>
@@ -1713,13 +1722,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="46"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="30">
         <v>20</v>
       </c>
@@ -1729,13 +1738,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="46"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="30">
         <v>45</v>
       </c>
@@ -1745,13 +1754,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="46"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="50"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="30">
         <v>55</v>
       </c>
@@ -1761,13 +1770,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="46"/>
+      <c r="G28" s="54"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="50"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="30">
         <v>70</v>
       </c>
@@ -1777,13 +1786,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="46"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="51"/>
+      <c r="C30" s="52"/>
       <c r="D30" s="30">
         <v>20</v>
       </c>
@@ -1793,7 +1802,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="47"/>
+      <c r="G30" s="55"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1814,7 +1823,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="52">
+      <c r="C32" s="50">
         <v>43595</v>
       </c>
       <c r="D32" s="30">
@@ -1826,7 +1835,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="53" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1834,7 +1843,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="50"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="30">
         <v>45</v>
       </c>
@@ -1844,13 +1853,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="46"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="50"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="30">
         <v>70</v>
       </c>
@@ -1860,13 +1869,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="46"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="50"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="30">
         <v>90</v>
       </c>
@@ -1876,13 +1885,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="46"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="50"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="30">
         <v>45</v>
       </c>
@@ -1892,13 +1901,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="46"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="50"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="30">
         <v>20</v>
       </c>
@@ -1908,13 +1917,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="46"/>
+      <c r="G37" s="54"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="51"/>
+      <c r="C38" s="52"/>
       <c r="D38" s="30">
         <v>25</v>
       </c>
@@ -1924,7 +1933,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="47"/>
+      <c r="G38" s="55"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -1945,7 +1954,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="52">
+      <c r="C40" s="50">
         <v>43599</v>
       </c>
       <c r="D40" s="30">
@@ -1957,7 +1966,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="48" t="s">
+      <c r="G40" s="53" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -1965,7 +1974,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="50"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="30">
         <v>15</v>
       </c>
@@ -1975,13 +1984,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="46"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="50"/>
+      <c r="C42" s="51"/>
       <c r="D42" s="30">
         <v>45</v>
       </c>
@@ -1991,13 +2000,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="46"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="50"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="30">
         <v>45</v>
       </c>
@@ -2007,13 +2016,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="46"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="50"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="30">
         <v>45</v>
       </c>
@@ -2023,13 +2032,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="46"/>
+      <c r="G44" s="54"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="50"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="30">
         <v>45</v>
       </c>
@@ -2039,13 +2048,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="46"/>
+      <c r="G45" s="54"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="50"/>
+      <c r="C46" s="51"/>
       <c r="D46" s="30">
         <v>45</v>
       </c>
@@ -2055,13 +2064,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="46"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="50"/>
+      <c r="C47" s="51"/>
       <c r="D47" s="30">
         <v>45</v>
       </c>
@@ -2071,13 +2080,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="46"/>
+      <c r="G47" s="54"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="50"/>
+      <c r="C48" s="51"/>
       <c r="D48" s="30">
         <v>15</v>
       </c>
@@ -2087,13 +2096,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="46"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="50"/>
+      <c r="C49" s="51"/>
       <c r="D49" s="30">
         <v>30</v>
       </c>
@@ -2103,13 +2112,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="46"/>
+      <c r="G49" s="54"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="51"/>
+      <c r="C50" s="52"/>
       <c r="D50" s="30">
         <v>45</v>
       </c>
@@ -2119,7 +2128,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="47"/>
+      <c r="G50" s="55"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
@@ -2140,7 +2149,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="52">
+      <c r="C52" s="50">
         <v>43600</v>
       </c>
       <c r="D52" s="30">
@@ -2152,7 +2161,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="54" t="s">
+      <c r="G52" s="57" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="23"/>
@@ -2160,7 +2169,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="50"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="30">
         <v>60</v>
       </c>
@@ -2170,13 +2179,13 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="55"/>
+      <c r="G53" s="58"/>
       <c r="H53" s="23"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="50"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="30">
         <v>45</v>
       </c>
@@ -2186,13 +2195,13 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="55"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="23"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="50"/>
+      <c r="C55" s="51"/>
       <c r="D55" s="30">
         <v>15</v>
       </c>
@@ -2202,13 +2211,13 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="55"/>
+      <c r="G55" s="58"/>
       <c r="H55" s="23"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="51"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="30">
         <v>45</v>
       </c>
@@ -2218,7 +2227,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="56"/>
+      <c r="G56" s="59"/>
       <c r="H56" s="23"/>
       <c r="I56" s="5"/>
     </row>
@@ -2239,7 +2248,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="52">
+      <c r="C58" s="50">
         <v>43601</v>
       </c>
       <c r="D58" s="30">
@@ -2251,7 +2260,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="48" t="s">
+      <c r="G58" s="53" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="23"/>
@@ -2259,7 +2268,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="50"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="30">
         <v>15</v>
       </c>
@@ -2269,13 +2278,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="46"/>
+      <c r="G59" s="54"/>
       <c r="H59" s="23"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="50"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="30">
         <v>45</v>
       </c>
@@ -2285,13 +2294,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="46"/>
+      <c r="G60" s="54"/>
       <c r="H60" s="23"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="50"/>
+      <c r="C61" s="51"/>
       <c r="D61" s="30">
         <v>90</v>
       </c>
@@ -2301,29 +2310,29 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="46"/>
+      <c r="G61" s="54"/>
       <c r="H61" s="23"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="58">
+      <c r="C62" s="51"/>
+      <c r="D62" s="45">
         <v>30</v>
       </c>
-      <c r="E62" s="59" t="s">
+      <c r="E62" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F62" s="60" t="s">
+      <c r="F62" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="46"/>
-      <c r="H62" s="62"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="49"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="50"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="30">
         <v>15</v>
       </c>
@@ -2333,13 +2342,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="46"/>
+      <c r="G63" s="54"/>
       <c r="H63" s="23"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="50"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="30">
         <v>45</v>
       </c>
@@ -2349,13 +2358,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="46"/>
+      <c r="G64" s="54"/>
       <c r="H64" s="23"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="50"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="30">
         <v>45</v>
       </c>
@@ -2365,13 +2374,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="46"/>
+      <c r="G65" s="54"/>
       <c r="H65" s="23"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="51"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="30">
         <v>90</v>
       </c>
@@ -2381,7 +2390,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="47"/>
+      <c r="G66" s="55"/>
       <c r="H66" s="23"/>
       <c r="I66" s="5"/>
     </row>
@@ -2390,34 +2399,50 @@
       <c r="C67" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D67" s="58">
+      <c r="D67" s="45">
         <f>SUM(D58:D66)</f>
         <v>405</v>
       </c>
-      <c r="E67" s="59"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="61"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="48"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="14"/>
+      <c r="C68" s="21">
+        <v>43602</v>
+      </c>
+      <c r="D68" s="30">
+        <v>45</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="G68" s="30"/>
-      <c r="H68" s="24"/>
+      <c r="H68" s="23"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="14"/>
+      <c r="C69" s="21">
+        <v>43602</v>
+      </c>
+      <c r="D69" s="30">
+        <v>45</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="G69" s="30"/>
-      <c r="H69" s="24"/>
+      <c r="H69" s="23"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
@@ -2442,12 +2467,12 @@
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="61"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="48"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
@@ -2492,33 +2517,78 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="59"/>
-      <c r="F77" s="60"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="61"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="46"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="48"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="8"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="45"/>
+      <c r="H78" s="48"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="4"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="4"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="4"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="30"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="8"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="9"/>
+    </row>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G52:G56"/>
@@ -2531,6 +2601,11 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Création de la page d'un jour précis
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
   <si>
     <t>Activités</t>
   </si>
@@ -369,6 +369,27 @@
   </si>
   <si>
     <t>Relecture de ma planification détaillée + insertion de celle-ci dans mon rapport de projet et relecture de toute mon analyse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diego Sanchez et Frédérique Andolfatto, Review </t>
+  </si>
+  <si>
+    <t>Petite présentation de mon avancé sur le code depuis le début du projet</t>
+  </si>
+  <si>
+    <t>Création de la page pour afficher un jour précis depuis un clic sur le calendrier, beaucoup de problème pour obtenir la date précise avec la variable du calendrier</t>
+  </si>
+  <si>
+    <t>Création de quelques tests pour le bon environnement de mon site, test de données avant de valider certains envoie ou insertion</t>
+  </si>
+  <si>
+    <t>Recherche de solutions afin de créer ma page pour afficher un jour précis depuis les variables de mon calendrier</t>
+  </si>
+  <si>
+    <t>Passablement de problèmes par rapport à mon code, mais j'ai trouvé les solutions à mes problèmes avec un petit peu de retard sur mon planning du jour.</t>
+  </si>
+  <si>
+    <t>17.05.2019, total durée</t>
   </si>
 </sst>
 </file>
@@ -849,7 +870,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -858,34 +906,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1360,31 +1381,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="56"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1446,7 +1467,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="62">
+      <c r="C9" s="59">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1458,7 +1479,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="55" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1466,7 +1487,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="30">
         <v>75</v>
       </c>
@@ -1476,13 +1497,13 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="54"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="51"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="30">
         <v>45</v>
       </c>
@@ -1492,13 +1513,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="54"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="30">
         <v>75</v>
       </c>
@@ -1508,13 +1529,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="54"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="51"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="30">
         <v>15</v>
       </c>
@@ -1524,13 +1545,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="54"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="30">
         <v>30</v>
       </c>
@@ -1540,13 +1561,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="51"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="30">
         <v>75</v>
       </c>
@@ -1556,13 +1577,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="52"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="30">
         <v>30</v>
       </c>
@@ -1572,7 +1593,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1593,7 +1614,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="50">
+      <c r="C18" s="62">
         <v>43593</v>
       </c>
       <c r="D18" s="30">
@@ -1605,7 +1626,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="58" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1613,7 +1634,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="30">
         <v>90</v>
       </c>
@@ -1623,13 +1644,13 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="54"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="52"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="30">
         <v>45</v>
       </c>
@@ -1639,7 +1660,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="55"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1660,7 +1681,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="50">
+      <c r="C22" s="62">
         <v>43594</v>
       </c>
       <c r="D22" s="30">
@@ -1672,7 +1693,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="58" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1680,7 +1701,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="51"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="30">
         <v>30</v>
       </c>
@@ -1690,13 +1711,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="56"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="51"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="30">
         <v>70</v>
       </c>
@@ -1706,13 +1727,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="56"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="51"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="30">
         <v>35</v>
       </c>
@@ -1722,13 +1743,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="54"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="51"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="30">
         <v>20</v>
       </c>
@@ -1738,13 +1759,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="54"/>
+      <c r="G26" s="56"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="51"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="30">
         <v>45</v>
       </c>
@@ -1754,13 +1775,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="56"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="51"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="30">
         <v>55</v>
       </c>
@@ -1770,13 +1791,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="54"/>
+      <c r="G28" s="56"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="51"/>
+      <c r="C29" s="60"/>
       <c r="D29" s="30">
         <v>70</v>
       </c>
@@ -1786,13 +1807,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="54"/>
+      <c r="G29" s="56"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="52"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="30">
         <v>20</v>
       </c>
@@ -1802,7 +1823,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="55"/>
+      <c r="G30" s="57"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1823,7 +1844,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="50">
+      <c r="C32" s="62">
         <v>43595</v>
       </c>
       <c r="D32" s="30">
@@ -1835,7 +1856,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="58" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1843,7 +1864,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="51"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="30">
         <v>45</v>
       </c>
@@ -1853,13 +1874,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="54"/>
+      <c r="G33" s="56"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="51"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="30">
         <v>70</v>
       </c>
@@ -1869,13 +1890,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="54"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="51"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="30">
         <v>90</v>
       </c>
@@ -1885,13 +1906,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="56"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="51"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="30">
         <v>45</v>
       </c>
@@ -1901,13 +1922,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="54"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="51"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="30">
         <v>20</v>
       </c>
@@ -1917,13 +1938,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="54"/>
+      <c r="G37" s="56"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="52"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="30">
         <v>25</v>
       </c>
@@ -1933,7 +1954,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="55"/>
+      <c r="G38" s="57"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -1954,7 +1975,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="50">
+      <c r="C40" s="62">
         <v>43599</v>
       </c>
       <c r="D40" s="30">
@@ -1966,7 +1987,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="58" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -1974,7 +1995,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="51"/>
+      <c r="C41" s="60"/>
       <c r="D41" s="30">
         <v>15</v>
       </c>
@@ -1984,13 +2005,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="54"/>
+      <c r="G41" s="56"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="51"/>
+      <c r="C42" s="60"/>
       <c r="D42" s="30">
         <v>45</v>
       </c>
@@ -2000,13 +2021,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="54"/>
+      <c r="G42" s="56"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="51"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="30">
         <v>45</v>
       </c>
@@ -2016,13 +2037,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="54"/>
+      <c r="G43" s="56"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="51"/>
+      <c r="C44" s="60"/>
       <c r="D44" s="30">
         <v>45</v>
       </c>
@@ -2032,13 +2053,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="54"/>
+      <c r="G44" s="56"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="51"/>
+      <c r="C45" s="60"/>
       <c r="D45" s="30">
         <v>45</v>
       </c>
@@ -2048,13 +2069,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="54"/>
+      <c r="G45" s="56"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="51"/>
+      <c r="C46" s="60"/>
       <c r="D46" s="30">
         <v>45</v>
       </c>
@@ -2064,13 +2085,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="54"/>
+      <c r="G46" s="56"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="51"/>
+      <c r="C47" s="60"/>
       <c r="D47" s="30">
         <v>45</v>
       </c>
@@ -2080,13 +2101,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="54"/>
+      <c r="G47" s="56"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="51"/>
+      <c r="C48" s="60"/>
       <c r="D48" s="30">
         <v>15</v>
       </c>
@@ -2096,13 +2117,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="54"/>
+      <c r="G48" s="56"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="51"/>
+      <c r="C49" s="60"/>
       <c r="D49" s="30">
         <v>30</v>
       </c>
@@ -2112,13 +2133,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="54"/>
+      <c r="G49" s="56"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="52"/>
+      <c r="C50" s="61"/>
       <c r="D50" s="30">
         <v>45</v>
       </c>
@@ -2128,7 +2149,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="55"/>
+      <c r="G50" s="57"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
@@ -2149,7 +2170,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="50">
+      <c r="C52" s="62">
         <v>43600</v>
       </c>
       <c r="D52" s="30">
@@ -2161,7 +2182,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="57" t="s">
+      <c r="G52" s="51" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="23"/>
@@ -2169,7 +2190,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="51"/>
+      <c r="C53" s="60"/>
       <c r="D53" s="30">
         <v>60</v>
       </c>
@@ -2179,13 +2200,13 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="58"/>
+      <c r="G53" s="52"/>
       <c r="H53" s="23"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="51"/>
+      <c r="C54" s="60"/>
       <c r="D54" s="30">
         <v>45</v>
       </c>
@@ -2195,13 +2216,13 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="58"/>
+      <c r="G54" s="52"/>
       <c r="H54" s="23"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="51"/>
+      <c r="C55" s="60"/>
       <c r="D55" s="30">
         <v>15</v>
       </c>
@@ -2211,13 +2232,13 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="58"/>
+      <c r="G55" s="52"/>
       <c r="H55" s="23"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="52"/>
+      <c r="C56" s="61"/>
       <c r="D56" s="30">
         <v>45</v>
       </c>
@@ -2227,7 +2248,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="59"/>
+      <c r="G56" s="53"/>
       <c r="H56" s="23"/>
       <c r="I56" s="5"/>
     </row>
@@ -2248,7 +2269,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="50">
+      <c r="C58" s="62">
         <v>43601</v>
       </c>
       <c r="D58" s="30">
@@ -2260,7 +2281,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="53" t="s">
+      <c r="G58" s="58" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="23"/>
@@ -2268,7 +2289,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="51"/>
+      <c r="C59" s="60"/>
       <c r="D59" s="30">
         <v>15</v>
       </c>
@@ -2278,13 +2299,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="54"/>
+      <c r="G59" s="56"/>
       <c r="H59" s="23"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="51"/>
+      <c r="C60" s="60"/>
       <c r="D60" s="30">
         <v>45</v>
       </c>
@@ -2294,13 +2315,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="54"/>
+      <c r="G60" s="56"/>
       <c r="H60" s="23"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="51"/>
+      <c r="C61" s="60"/>
       <c r="D61" s="30">
         <v>90</v>
       </c>
@@ -2310,13 +2331,13 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="54"/>
+      <c r="G61" s="56"/>
       <c r="H61" s="23"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="51"/>
+      <c r="C62" s="60"/>
       <c r="D62" s="45">
         <v>30</v>
       </c>
@@ -2326,13 +2347,13 @@
       <c r="F62" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="54"/>
+      <c r="G62" s="56"/>
       <c r="H62" s="49"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="51"/>
+      <c r="C63" s="60"/>
       <c r="D63" s="30">
         <v>15</v>
       </c>
@@ -2342,13 +2363,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="54"/>
+      <c r="G63" s="56"/>
       <c r="H63" s="23"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="51"/>
+      <c r="C64" s="60"/>
       <c r="D64" s="30">
         <v>45</v>
       </c>
@@ -2358,13 +2379,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="54"/>
+      <c r="G64" s="56"/>
       <c r="H64" s="23"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="51"/>
+      <c r="C65" s="60"/>
       <c r="D65" s="30">
         <v>45</v>
       </c>
@@ -2374,13 +2395,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="54"/>
+      <c r="G65" s="56"/>
       <c r="H65" s="23"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="52"/>
+      <c r="C66" s="61"/>
       <c r="D66" s="30">
         <v>90</v>
       </c>
@@ -2390,7 +2411,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="55"/>
+      <c r="G66" s="57"/>
       <c r="H66" s="23"/>
       <c r="I66" s="5"/>
     </row>
@@ -2411,7 +2432,7 @@
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="21">
+      <c r="C68" s="62">
         <v>43602</v>
       </c>
       <c r="D68" s="30">
@@ -2423,15 +2444,15 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="30"/>
+      <c r="G68" s="58" t="s">
+        <v>120</v>
+      </c>
       <c r="H68" s="23"/>
       <c r="I68" s="5"/>
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="21">
-        <v>43602</v>
-      </c>
+      <c r="C69" s="60"/>
       <c r="D69" s="30">
         <v>45</v>
       </c>
@@ -2441,54 +2462,83 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="56"/>
       <c r="H69" s="23"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="24"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="30">
+        <v>45</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G70" s="56"/>
+      <c r="H70" s="23"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="24"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="30">
+        <v>45</v>
+      </c>
+      <c r="E71" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="56"/>
+      <c r="H71" s="23"/>
       <c r="I71" s="5"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="48"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="45">
+        <v>45</v>
+      </c>
+      <c r="E72" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="G72" s="56"/>
+      <c r="H72" s="49"/>
       <c r="I72" s="5"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="24"/>
+      <c r="C73" s="61"/>
+      <c r="D73" s="30">
+        <v>90</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G73" s="57"/>
+      <c r="H73" s="23"/>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="30"/>
+      <c r="C74" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" s="30">
+        <f>SUM(D68:D73)</f>
+        <v>315</v>
+      </c>
       <c r="E74" s="25"/>
       <c r="F74" s="14"/>
       <c r="G74" s="30"/>
@@ -2507,12 +2557,12 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="24"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="48"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
@@ -2527,12 +2577,12 @@
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="48"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="30"/>
+      <c r="H78" s="24"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
@@ -2566,29 +2616,26 @@
       <c r="I81" s="5"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B82" s="4"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="24"/>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B83" s="8"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="9"/>
-    </row>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="9"/>
+    </row>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G52:G56"/>
@@ -2601,11 +2648,6 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Ajout rendez-vous et affichage vue d'une jour précis avec ces tâches et rendez-vous
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="130">
   <si>
     <t>Activités</t>
   </si>
@@ -390,6 +390,30 @@
   </si>
   <si>
     <t>17.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Mise en place des tests pour l'affichage de la date d'un jour précis.</t>
+  </si>
+  <si>
+    <t>Affichage des rendez-vous du jour en cliquant sur un jour précis</t>
+  </si>
+  <si>
+    <t>Affichage des tâches du jour en cliquant sur un jour précis</t>
+  </si>
+  <si>
+    <t>Ajout d'un rendez-vous grâce à une icône en cliquant sur un jour précis</t>
+  </si>
+  <si>
+    <t>Réglage de quelques tests et modification sur le formulaire d'ajout d'un rendez-vous.</t>
+  </si>
+  <si>
+    <t>21.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Recherche</t>
+  </si>
+  <si>
+    <t>Recherche de solutions, à cause d'un problème d'affichage de ma date dans ma BDD lors de l'affichage</t>
   </si>
 </sst>
 </file>
@@ -741,7 +765,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -852,9 +876,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -870,6 +891,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,25 +927,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1360,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M125"/>
+  <dimension ref="A1:M136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1381,31 +1402,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1467,7 +1488,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="59">
+      <c r="C9" s="61">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1479,7 +1500,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="60" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1487,7 +1508,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="60"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="30">
         <v>75</v>
       </c>
@@ -1497,13 +1518,13 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="60"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="30">
         <v>45</v>
       </c>
@@ -1513,13 +1534,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="56"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="60"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="30">
         <v>75</v>
       </c>
@@ -1529,13 +1550,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="56"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="60"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="30">
         <v>15</v>
       </c>
@@ -1545,13 +1566,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="56"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="60"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="30">
         <v>30</v>
       </c>
@@ -1561,13 +1582,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="56"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="60"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="30">
         <v>75</v>
       </c>
@@ -1577,13 +1598,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="53"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="61"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="30">
         <v>30</v>
       </c>
@@ -1593,7 +1614,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="57"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1614,7 +1635,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="62">
+      <c r="C18" s="49">
         <v>43593</v>
       </c>
       <c r="D18" s="30">
@@ -1626,7 +1647,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="58" t="s">
+      <c r="G18" s="52" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1634,7 +1655,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="60"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="30">
         <v>90</v>
       </c>
@@ -1644,13 +1665,13 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="56"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="61"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="30">
         <v>45</v>
       </c>
@@ -1660,7 +1681,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="57"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1681,7 +1702,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="62">
+      <c r="C22" s="49">
         <v>43594</v>
       </c>
       <c r="D22" s="30">
@@ -1693,7 +1714,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="52" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1701,7 +1722,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="60"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="30">
         <v>30</v>
       </c>
@@ -1711,13 +1732,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="56"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="60"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="30">
         <v>70</v>
       </c>
@@ -1727,13 +1748,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="56"/>
+      <c r="G24" s="53"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="60"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="30">
         <v>35</v>
       </c>
@@ -1743,13 +1764,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="56"/>
+      <c r="G25" s="53"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="60"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="30">
         <v>20</v>
       </c>
@@ -1759,13 +1780,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="56"/>
+      <c r="G26" s="53"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="60"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="30">
         <v>45</v>
       </c>
@@ -1775,13 +1796,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="56"/>
+      <c r="G27" s="53"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="60"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="30">
         <v>55</v>
       </c>
@@ -1791,13 +1812,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="56"/>
+      <c r="G28" s="53"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="60"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="30">
         <v>70</v>
       </c>
@@ -1807,13 +1828,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="56"/>
+      <c r="G29" s="53"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="61"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="30">
         <v>20</v>
       </c>
@@ -1823,7 +1844,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="57"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1844,7 +1865,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="62">
+      <c r="C32" s="49">
         <v>43595</v>
       </c>
       <c r="D32" s="30">
@@ -1856,7 +1877,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="58" t="s">
+      <c r="G32" s="52" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1864,7 +1885,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="60"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="30">
         <v>45</v>
       </c>
@@ -1874,13 +1895,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="56"/>
+      <c r="G33" s="53"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="60"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="30">
         <v>70</v>
       </c>
@@ -1890,13 +1911,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="56"/>
+      <c r="G34" s="53"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="60"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="30">
         <v>90</v>
       </c>
@@ -1906,13 +1927,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="56"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="60"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="30">
         <v>45</v>
       </c>
@@ -1922,13 +1943,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="56"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="60"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="30">
         <v>20</v>
       </c>
@@ -1938,13 +1959,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="56"/>
+      <c r="G37" s="53"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="61"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="30">
         <v>25</v>
       </c>
@@ -1954,7 +1975,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="57"/>
+      <c r="G38" s="54"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -1975,7 +1996,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="62">
+      <c r="C40" s="49">
         <v>43599</v>
       </c>
       <c r="D40" s="30">
@@ -1987,7 +2008,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="58" t="s">
+      <c r="G40" s="52" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -1995,7 +2016,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="60"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="30">
         <v>15</v>
       </c>
@@ -2005,13 +2026,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="56"/>
+      <c r="G41" s="53"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="60"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="30">
         <v>45</v>
       </c>
@@ -2021,13 +2042,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="56"/>
+      <c r="G42" s="53"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="60"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="30">
         <v>45</v>
       </c>
@@ -2037,13 +2058,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="56"/>
+      <c r="G43" s="53"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="60"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="30">
         <v>45</v>
       </c>
@@ -2053,13 +2074,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="56"/>
+      <c r="G44" s="53"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="60"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="30">
         <v>45</v>
       </c>
@@ -2069,13 +2090,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="56"/>
+      <c r="G45" s="53"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="60"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="30">
         <v>45</v>
       </c>
@@ -2085,13 +2106,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="56"/>
+      <c r="G46" s="53"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="60"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="30">
         <v>45</v>
       </c>
@@ -2101,13 +2122,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="56"/>
+      <c r="G47" s="53"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="60"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="30">
         <v>15</v>
       </c>
@@ -2117,13 +2138,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="56"/>
+      <c r="G48" s="53"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="60"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="30">
         <v>30</v>
       </c>
@@ -2133,13 +2154,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="56"/>
+      <c r="G49" s="53"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="61"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="30">
         <v>45</v>
       </c>
@@ -2149,7 +2170,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="57"/>
+      <c r="G50" s="54"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
@@ -2170,7 +2191,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="62">
+      <c r="C52" s="49">
         <v>43600</v>
       </c>
       <c r="D52" s="30">
@@ -2182,7 +2203,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="51" t="s">
+      <c r="G52" s="56" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="23"/>
@@ -2190,7 +2211,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="60"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="30">
         <v>60</v>
       </c>
@@ -2200,13 +2221,13 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="52"/>
+      <c r="G53" s="57"/>
       <c r="H53" s="23"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="60"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="30">
         <v>45</v>
       </c>
@@ -2216,13 +2237,13 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="52"/>
+      <c r="G54" s="57"/>
       <c r="H54" s="23"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="60"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="30">
         <v>15</v>
       </c>
@@ -2232,13 +2253,13 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="52"/>
+      <c r="G55" s="57"/>
       <c r="H55" s="23"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="61"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="30">
         <v>45</v>
       </c>
@@ -2248,7 +2269,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="53"/>
+      <c r="G56" s="58"/>
       <c r="H56" s="23"/>
       <c r="I56" s="5"/>
     </row>
@@ -2269,7 +2290,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="62">
+      <c r="C58" s="49">
         <v>43601</v>
       </c>
       <c r="D58" s="30">
@@ -2281,7 +2302,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="58" t="s">
+      <c r="G58" s="52" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="23"/>
@@ -2289,7 +2310,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="60"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="30">
         <v>15</v>
       </c>
@@ -2299,13 +2320,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="56"/>
+      <c r="G59" s="53"/>
       <c r="H59" s="23"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="60"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="30">
         <v>45</v>
       </c>
@@ -2315,13 +2336,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="56"/>
+      <c r="G60" s="53"/>
       <c r="H60" s="23"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="60"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="30">
         <v>90</v>
       </c>
@@ -2331,29 +2352,29 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="56"/>
+      <c r="G61" s="53"/>
       <c r="H61" s="23"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="60"/>
-      <c r="D62" s="45">
+      <c r="C62" s="50"/>
+      <c r="D62" s="44">
         <v>30</v>
       </c>
-      <c r="E62" s="46" t="s">
+      <c r="E62" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="F62" s="47" t="s">
+      <c r="F62" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="56"/>
-      <c r="H62" s="49"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="48"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="60"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="30">
         <v>15</v>
       </c>
@@ -2363,13 +2384,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="56"/>
+      <c r="G63" s="53"/>
       <c r="H63" s="23"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="60"/>
+      <c r="C64" s="50"/>
       <c r="D64" s="30">
         <v>45</v>
       </c>
@@ -2379,13 +2400,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="56"/>
+      <c r="G64" s="53"/>
       <c r="H64" s="23"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="60"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="30">
         <v>45</v>
       </c>
@@ -2395,13 +2416,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="56"/>
+      <c r="G65" s="53"/>
       <c r="H65" s="23"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="61"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="30">
         <v>90</v>
       </c>
@@ -2411,7 +2432,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="57"/>
+      <c r="G66" s="54"/>
       <c r="H66" s="23"/>
       <c r="I66" s="5"/>
     </row>
@@ -2420,19 +2441,19 @@
       <c r="C67" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D67" s="45">
+      <c r="D67" s="44">
         <f>SUM(D58:D66)</f>
         <v>405</v>
       </c>
-      <c r="E67" s="46"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="48"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="47"/>
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="62">
+      <c r="C68" s="49">
         <v>43602</v>
       </c>
       <c r="D68" s="30">
@@ -2444,7 +2465,7 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="58" t="s">
+      <c r="G68" s="52" t="s">
         <v>120</v>
       </c>
       <c r="H68" s="23"/>
@@ -2452,7 +2473,7 @@
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="60"/>
+      <c r="C69" s="50"/>
       <c r="D69" s="30">
         <v>45</v>
       </c>
@@ -2462,13 +2483,13 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="56"/>
+      <c r="G69" s="53"/>
       <c r="H69" s="23"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="60"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="30">
         <v>45</v>
       </c>
@@ -2478,45 +2499,45 @@
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="56"/>
+      <c r="G70" s="53"/>
       <c r="H70" s="23"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="60"/>
+      <c r="C71" s="50"/>
       <c r="D71" s="30">
         <v>45</v>
       </c>
-      <c r="E71" s="46" t="s">
+      <c r="E71" s="45" t="s">
         <v>71</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="56"/>
+      <c r="G71" s="53"/>
       <c r="H71" s="23"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="60"/>
-      <c r="D72" s="45">
+      <c r="C72" s="50"/>
+      <c r="D72" s="44">
         <v>45</v>
       </c>
-      <c r="E72" s="46" t="s">
+      <c r="E72" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="F72" s="47" t="s">
+      <c r="F72" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="56"/>
-      <c r="H72" s="49"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="48"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="61"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="30">
         <v>90</v>
       </c>
@@ -2526,7 +2547,7 @@
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="57"/>
+      <c r="G73" s="54"/>
       <c r="H73" s="23"/>
       <c r="I73" s="5"/>
     </row>
@@ -2545,70 +2566,113 @@
       <c r="H74" s="24"/>
       <c r="I74" s="5"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="14"/>
+      <c r="C75" s="49">
+        <v>43606</v>
+      </c>
+      <c r="D75" s="30">
+        <v>45</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>122</v>
+      </c>
       <c r="G75" s="30"/>
-      <c r="H75" s="24"/>
+      <c r="H75" s="23"/>
       <c r="I75" s="5"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="46"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="45"/>
+      <c r="C76" s="50"/>
+      <c r="D76" s="44">
+        <v>90</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F76" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G76" s="44"/>
       <c r="H76" s="48"/>
       <c r="I76" s="5"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="46"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="48"/>
+      <c r="C77" s="50"/>
+      <c r="D77" s="30">
+        <v>45</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G77" s="30"/>
+      <c r="H77" s="23"/>
       <c r="I77" s="5"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="24"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="44">
+        <v>90</v>
+      </c>
+      <c r="E78" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F78" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G78" s="44"/>
+      <c r="H78" s="48"/>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="14"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="30">
+        <v>90</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>125</v>
+      </c>
       <c r="G79" s="30"/>
-      <c r="H79" s="24"/>
+      <c r="H79" s="23"/>
       <c r="I79" s="5"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="14"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="30">
+        <v>45</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="G80" s="30"/>
-      <c r="H80" s="24"/>
+      <c r="H80" s="23"/>
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="30"/>
+      <c r="C81" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="30">
+        <f>SUM(D75:D80)</f>
+        <v>405</v>
+      </c>
       <c r="E81" s="25"/>
       <c r="F81" s="14"/>
       <c r="G81" s="30"/>
@@ -2616,29 +2680,130 @@
       <c r="I81" s="5"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B82" s="8"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="9"/>
-    </row>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="30"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="4"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="30"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="4"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="4"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="4"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="30"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="4"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B88" s="4"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="30"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B89" s="4"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="30"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90" s="4"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="4"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B92" s="4"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="30"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B93" s="8"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="9"/>
+    </row>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C68:C73"/>
-    <mergeCell ref="G68:G73"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
+  <mergeCells count="20">
+    <mergeCell ref="C75:C80"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -2648,6 +2813,16 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C52:C56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Début de l'affichage par semaine
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="138">
   <si>
     <t>Activités</t>
   </si>
@@ -414,6 +414,30 @@
   </si>
   <si>
     <t>Recherche de solutions, à cause d'un problème d'affichage de ma date dans ma BDD lors de l'affichage</t>
+  </si>
+  <si>
+    <t>Diego Sanchez,Code</t>
+  </si>
+  <si>
+    <t>Mise en place de l'ajout des tâches</t>
+  </si>
+  <si>
+    <t>Création de la page Mes tâches et rendez-vous qui affiche toutes les tâches et les rendez-vous de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Début de l'affichage par semaine de mon calendrier, passablement de problème pour l'affichage par semaine, pour obtenir la semaine actuelle grâce à la date du jour</t>
+  </si>
+  <si>
+    <t>Recherche de solution pour régler mon problème d'affichage par semaine de mon calendrier</t>
+  </si>
+  <si>
+    <t>22.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Bonne avancée de mon code mais quelques problèmes m'ont bloqué</t>
+  </si>
+  <si>
+    <t>Je suis bloqué sur un problème d'affichage et je pense perdre trop de temps même si je suis plutôt bien dans les temps avec mon projet</t>
   </si>
 </sst>
 </file>
@@ -900,13 +924,22 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -919,15 +952,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1381,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M136"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1402,31 +1426,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="55"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1488,7 +1512,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="61">
+      <c r="C9" s="57">
         <v>43592</v>
       </c>
       <c r="D9" s="40">
@@ -1500,7 +1524,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="53" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1518,7 +1542,7 @@
       <c r="F10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="53"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="23"/>
       <c r="I10" s="5"/>
     </row>
@@ -1534,7 +1558,7 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="53"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="23"/>
       <c r="I11" s="5"/>
     </row>
@@ -1550,7 +1574,7 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="23"/>
       <c r="I12" s="5"/>
     </row>
@@ -1566,7 +1590,7 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="53"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="23"/>
       <c r="I13" s="5"/>
     </row>
@@ -1582,7 +1606,7 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="23"/>
       <c r="I14" s="5"/>
     </row>
@@ -1598,7 +1622,7 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="23"/>
       <c r="I15" s="5"/>
     </row>
@@ -1614,7 +1638,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="23"/>
       <c r="I16" s="5"/>
     </row>
@@ -1647,7 +1671,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="56" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="23"/>
@@ -1665,7 +1689,7 @@
       <c r="F19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="23"/>
       <c r="I19" s="5"/>
     </row>
@@ -1681,7 +1705,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="23"/>
       <c r="I20" s="5"/>
     </row>
@@ -1714,7 +1738,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="56" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="23"/>
@@ -1732,7 +1756,7 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="53"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="23"/>
       <c r="I23" s="5"/>
     </row>
@@ -1748,7 +1772,7 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="53"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="23"/>
       <c r="I24" s="5"/>
     </row>
@@ -1764,7 +1788,7 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="53"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="23"/>
       <c r="I25" s="5"/>
     </row>
@@ -1780,7 +1804,7 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="53"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="23"/>
       <c r="I26" s="5"/>
     </row>
@@ -1796,7 +1820,7 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="53"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="23"/>
       <c r="I27" s="5"/>
     </row>
@@ -1812,7 +1836,7 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="53"/>
+      <c r="G28" s="54"/>
       <c r="H28" s="23"/>
       <c r="I28" s="5"/>
     </row>
@@ -1828,7 +1852,7 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="53"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="23"/>
       <c r="I29" s="5"/>
     </row>
@@ -1844,7 +1868,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="55"/>
       <c r="H30" s="23"/>
       <c r="I30" s="5"/>
     </row>
@@ -1877,7 +1901,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="52" t="s">
+      <c r="G32" s="56" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="23"/>
@@ -1895,7 +1919,7 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="53"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="23"/>
       <c r="I33" s="5"/>
     </row>
@@ -1911,7 +1935,7 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="53"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="23"/>
       <c r="I34" s="5"/>
     </row>
@@ -1927,7 +1951,7 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="53"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="23"/>
       <c r="I35" s="5"/>
     </row>
@@ -1943,7 +1967,7 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="53"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="23"/>
       <c r="I36" s="5"/>
     </row>
@@ -1959,7 +1983,7 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="53"/>
+      <c r="G37" s="54"/>
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
@@ -1975,7 +1999,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="54"/>
+      <c r="G38" s="55"/>
       <c r="H38" s="23"/>
       <c r="I38" s="5"/>
     </row>
@@ -2008,7 +2032,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="52" t="s">
+      <c r="G40" s="56" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="23"/>
@@ -2026,7 +2050,7 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="53"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="23"/>
       <c r="I41" s="5"/>
     </row>
@@ -2042,7 +2066,7 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="53"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="23"/>
       <c r="I42" s="5"/>
     </row>
@@ -2058,7 +2082,7 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="23"/>
       <c r="I43" s="5"/>
     </row>
@@ -2074,7 +2098,7 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="53"/>
+      <c r="G44" s="54"/>
       <c r="H44" s="23"/>
       <c r="I44" s="5"/>
     </row>
@@ -2090,7 +2114,7 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="53"/>
+      <c r="G45" s="54"/>
       <c r="H45" s="23"/>
       <c r="I45" s="5"/>
     </row>
@@ -2106,7 +2130,7 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="53"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="23"/>
       <c r="I46" s="5"/>
     </row>
@@ -2122,7 +2146,7 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="53"/>
+      <c r="G47" s="54"/>
       <c r="H47" s="23"/>
       <c r="I47" s="5"/>
     </row>
@@ -2138,7 +2162,7 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="53"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="23"/>
       <c r="I48" s="5"/>
     </row>
@@ -2154,7 +2178,7 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="53"/>
+      <c r="G49" s="54"/>
       <c r="H49" s="23"/>
       <c r="I49" s="5"/>
     </row>
@@ -2170,7 +2194,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="54"/>
+      <c r="G50" s="55"/>
       <c r="H50" s="23"/>
       <c r="I50" s="5"/>
     </row>
@@ -2203,7 +2227,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="56" t="s">
+      <c r="G52" s="59" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="23"/>
@@ -2221,7 +2245,7 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="57"/>
+      <c r="G53" s="60"/>
       <c r="H53" s="23"/>
       <c r="I53" s="5"/>
     </row>
@@ -2237,7 +2261,7 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="57"/>
+      <c r="G54" s="60"/>
       <c r="H54" s="23"/>
       <c r="I54" s="5"/>
     </row>
@@ -2253,7 +2277,7 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="57"/>
+      <c r="G55" s="60"/>
       <c r="H55" s="23"/>
       <c r="I55" s="5"/>
     </row>
@@ -2269,7 +2293,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="58"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="23"/>
       <c r="I56" s="5"/>
     </row>
@@ -2302,7 +2326,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="52" t="s">
+      <c r="G58" s="56" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="23"/>
@@ -2320,7 +2344,7 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="53"/>
+      <c r="G59" s="54"/>
       <c r="H59" s="23"/>
       <c r="I59" s="5"/>
     </row>
@@ -2336,7 +2360,7 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="53"/>
+      <c r="G60" s="54"/>
       <c r="H60" s="23"/>
       <c r="I60" s="5"/>
     </row>
@@ -2352,7 +2376,7 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="53"/>
+      <c r="G61" s="54"/>
       <c r="H61" s="23"/>
       <c r="I61" s="5"/>
     </row>
@@ -2368,7 +2392,7 @@
       <c r="F62" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="53"/>
+      <c r="G62" s="54"/>
       <c r="H62" s="48"/>
       <c r="I62" s="5"/>
     </row>
@@ -2384,7 +2408,7 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="53"/>
+      <c r="G63" s="54"/>
       <c r="H63" s="23"/>
       <c r="I63" s="5"/>
     </row>
@@ -2400,7 +2424,7 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="53"/>
+      <c r="G64" s="54"/>
       <c r="H64" s="23"/>
       <c r="I64" s="5"/>
     </row>
@@ -2416,7 +2440,7 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="53"/>
+      <c r="G65" s="54"/>
       <c r="H65" s="23"/>
       <c r="I65" s="5"/>
     </row>
@@ -2432,7 +2456,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="54"/>
+      <c r="G66" s="55"/>
       <c r="H66" s="23"/>
       <c r="I66" s="5"/>
     </row>
@@ -2465,7 +2489,7 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="52" t="s">
+      <c r="G68" s="56" t="s">
         <v>120</v>
       </c>
       <c r="H68" s="23"/>
@@ -2483,7 +2507,7 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="53"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="23"/>
       <c r="I69" s="5"/>
     </row>
@@ -2499,7 +2523,7 @@
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="53"/>
+      <c r="G70" s="54"/>
       <c r="H70" s="23"/>
       <c r="I70" s="5"/>
     </row>
@@ -2515,7 +2539,7 @@
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="53"/>
+      <c r="G71" s="54"/>
       <c r="H71" s="23"/>
       <c r="I71" s="5"/>
     </row>
@@ -2531,7 +2555,7 @@
       <c r="F72" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="53"/>
+      <c r="G72" s="54"/>
       <c r="H72" s="48"/>
       <c r="I72" s="5"/>
     </row>
@@ -2547,7 +2571,7 @@
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="54"/>
+      <c r="G73" s="55"/>
       <c r="H73" s="23"/>
       <c r="I73" s="5"/>
     </row>
@@ -2580,7 +2604,9 @@
       <c r="F75" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G75" s="30"/>
+      <c r="G75" s="56" t="s">
+        <v>136</v>
+      </c>
       <c r="H75" s="23"/>
       <c r="I75" s="5"/>
     </row>
@@ -2596,7 +2622,7 @@
       <c r="F76" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="44"/>
+      <c r="G76" s="54"/>
       <c r="H76" s="48"/>
       <c r="I76" s="5"/>
     </row>
@@ -2612,7 +2638,7 @@
       <c r="F77" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="30"/>
+      <c r="G77" s="54"/>
       <c r="H77" s="23"/>
       <c r="I77" s="5"/>
     </row>
@@ -2628,7 +2654,7 @@
       <c r="F78" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="G78" s="44"/>
+      <c r="G78" s="54"/>
       <c r="H78" s="48"/>
       <c r="I78" s="5"/>
     </row>
@@ -2644,7 +2670,7 @@
       <c r="F79" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="30"/>
+      <c r="G79" s="54"/>
       <c r="H79" s="23"/>
       <c r="I79" s="5"/>
     </row>
@@ -2660,7 +2686,7 @@
       <c r="F80" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G80" s="30"/>
+      <c r="G80" s="55"/>
       <c r="H80" s="23"/>
       <c r="I80" s="5"/>
     </row>
@@ -2679,50 +2705,83 @@
       <c r="H81" s="24"/>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="24"/>
+      <c r="C82" s="49">
+        <v>43607</v>
+      </c>
+      <c r="D82" s="30">
+        <v>45</v>
+      </c>
+      <c r="E82" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G82" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="H82" s="23"/>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="30"/>
-      <c r="H83" s="24"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="30">
+        <v>45</v>
+      </c>
+      <c r="E83" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G83" s="60"/>
+      <c r="H83" s="23"/>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="30"/>
-      <c r="H84" s="24"/>
+      <c r="C84" s="50"/>
+      <c r="D84" s="30">
+        <v>90</v>
+      </c>
+      <c r="E84" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G84" s="60"/>
+      <c r="H84" s="23"/>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="30"/>
-      <c r="H85" s="24"/>
+      <c r="C85" s="50"/>
+      <c r="D85" s="30">
+        <v>45</v>
+      </c>
+      <c r="E85" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G85" s="61"/>
+      <c r="H85" s="23"/>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="4"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="30"/>
+      <c r="C86" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D86" s="30">
+        <f>SUM(D82:D85)</f>
+        <v>225</v>
+      </c>
       <c r="E86" s="25"/>
       <c r="F86" s="14"/>
       <c r="G86" s="30"/>
@@ -2740,69 +2799,26 @@
       <c r="I87" s="5"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B88" s="4"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="30"/>
-      <c r="H88" s="24"/>
-      <c r="I88" s="5"/>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B89" s="4"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="30"/>
-      <c r="H89" s="24"/>
-      <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B90" s="4"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="24"/>
-      <c r="I90" s="5"/>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B91" s="4"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="30"/>
-      <c r="H91" s="24"/>
-      <c r="I91" s="5"/>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B92" s="4"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="30"/>
-      <c r="H92" s="24"/>
-      <c r="I92" s="5"/>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B93" s="8"/>
-      <c r="C93" s="22"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="19"/>
-      <c r="I93" s="9"/>
-    </row>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="9"/>
+    </row>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="G75:G80"/>
+    <mergeCell ref="G82:G85"/>
     <mergeCell ref="C75:C80"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
@@ -2819,10 +2835,6 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G52:G56"/>
     <mergeCell ref="C68:C73"/>
-    <mergeCell ref="G68:G73"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C52:C56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Mise en place de la validation par mail ainsi que divers avancement du code
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
   <si>
     <t>Activités</t>
   </si>
@@ -438,6 +438,66 @@
   </si>
   <si>
     <t>Je suis bloqué sur un problème d'affichage et je pense perdre trop de temps même si je suis plutôt bien dans les temps avec mon projet</t>
+  </si>
+  <si>
+    <t>Création de la vue d'affichage pour administrateur de la liste de tous les utilisateurs</t>
+  </si>
+  <si>
+    <t>Création de la suppression d'une tâches et d'un meeting</t>
+  </si>
+  <si>
+    <t>Création de la modification d'une tâches via la vue d'un jour selectionné</t>
+  </si>
+  <si>
+    <t>Création de la modification d'un rendez-vous via la vue d'un jour selectionné</t>
+  </si>
+  <si>
+    <t>Création de la partie de paramétrage de mon application</t>
+  </si>
+  <si>
+    <t>Réalisation de quelques tests d'intégration afin de tester l'état actuel de mon application</t>
+  </si>
+  <si>
+    <t>Réglage des quelques problèmes que j'ai trouvé suite à mes tests sur mon application.</t>
+  </si>
+  <si>
+    <t>23.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>J'ai laissé mon problème d'affichage de coté afin de me concentrer sur le reste de mon projet. Grosse avancée dans les objectifs de mon cahier des charges.</t>
+  </si>
+  <si>
+    <t>Diego Sanchez et Sueleyman Ceran, Visite</t>
+  </si>
+  <si>
+    <t>2ème visite d'expert réalisé par mon expert numéro 2, nous avons parlé de l'avancé de nos projets ainsi que quelques notifications pour le rendu et la présentation</t>
+  </si>
+  <si>
+    <t>Mise au propre de mes notes prises durant la venu de Mr Ceran.</t>
+  </si>
+  <si>
+    <t>Review avec ma cheffe de projet afin de lui faire une démo de mon application, nous avons discuté de mon avancée tout au lieu de ce projet, et elle m'a suggérer des modifications et des conseils que je pourrais mettre en place afin d'améliorer mon code</t>
+  </si>
+  <si>
+    <t>Réglage des quelques problèmes trouvés lors de la review avec ma cheffe de projet</t>
+  </si>
+  <si>
+    <t>Mise en place de l'envoi de mail de mon application, test et recherche afin de continuer mon projet</t>
+  </si>
+  <si>
+    <t>Mise en place de la validation de compte par mail afin que les utilisateurs puissent se valider eux même</t>
+  </si>
+  <si>
+    <t>Rédaction de mon journal de bord</t>
+  </si>
+  <si>
+    <t>Divers petits réglage de mon application trouvé au fil et à mesure de tester mon site</t>
+  </si>
+  <si>
+    <t>24.05.2019, total durée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonne avancée avec la mise en place de la validation de compte par mail. </t>
   </si>
 </sst>
 </file>
@@ -789,7 +849,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -828,9 +888,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -924,35 +981,35 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1405,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M131"/>
+  <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1416,48 +1473,48 @@
     <col min="1" max="1" width="2.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18" style="31" customWidth="1"/>
+    <col min="4" max="4" width="18" style="30" customWidth="1"/>
     <col min="5" max="5" width="48.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="51.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="31" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="30" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" customWidth="1"/>
     <col min="9" max="9" width="1.28515625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
-      <c r="D5" s="32"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="32"/>
+      <c r="G5" s="31"/>
       <c r="H5" s="3"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -1467,9 +1524,9 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="32"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="1"/>
       <c r="I6" s="7"/>
     </row>
@@ -1477,14 +1534,14 @@
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="34"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="33" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -1497,7 +1554,7 @@
       <c r="C8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="12" t="s">
@@ -1506,25 +1563,25 @@
       <c r="F8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="12"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="57">
+      <c r="C9" s="59">
         <v>43592</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>15</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="58" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1532,1294 +1589,1561 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="30">
+      <c r="C10" s="49"/>
+      <c r="D10" s="29">
         <v>75</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="30">
-        <v>45</v>
-      </c>
-      <c r="E11" s="25" t="s">
+      <c r="C11" s="49"/>
+      <c r="D11" s="29">
+        <v>45</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="54"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="30">
+      <c r="C12" s="49"/>
+      <c r="D12" s="29">
         <v>75</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="30">
+      <c r="C13" s="49"/>
+      <c r="D13" s="29">
         <v>15</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="54"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="30">
+      <c r="C14" s="49"/>
+      <c r="D14" s="29">
         <v>30</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="54"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="30">
+      <c r="C15" s="49"/>
+      <c r="D15" s="29">
         <v>75</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="30">
+      <c r="C16" s="50"/>
+      <c r="D16" s="29">
         <v>30</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="41">
         <f>SUM(D9:D16)</f>
         <v>360</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="23"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="49">
+      <c r="C18" s="48">
         <v>43593</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="29">
         <v>90</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="30">
+      <c r="C19" s="49"/>
+      <c r="D19" s="29">
         <v>90</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="30">
-        <v>45</v>
-      </c>
-      <c r="E20" s="28" t="s">
+      <c r="C20" s="50"/>
+      <c r="D20" s="29">
+        <v>45</v>
+      </c>
+      <c r="E20" s="27" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="23"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="29">
         <f>SUM(D18:D20)</f>
         <v>225</v>
       </c>
-      <c r="E21" s="28"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="24"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="49">
+      <c r="C22" s="48">
         <v>43594</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="29">
         <v>60</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="56" t="s">
+      <c r="G22" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="23"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="30">
+      <c r="C23" s="49"/>
+      <c r="D23" s="29">
         <v>30</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="54"/>
-      <c r="H23" s="23"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="30">
+      <c r="C24" s="49"/>
+      <c r="D24" s="29">
         <v>70</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="54"/>
-      <c r="H24" s="23"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="30">
+      <c r="C25" s="49"/>
+      <c r="D25" s="29">
         <v>35</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="54"/>
-      <c r="H25" s="23"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="30">
+      <c r="C26" s="49"/>
+      <c r="D26" s="29">
         <v>20</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="23"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="30">
-        <v>45</v>
-      </c>
-      <c r="E27" s="25" t="s">
+      <c r="C27" s="49"/>
+      <c r="D27" s="29">
+        <v>45</v>
+      </c>
+      <c r="E27" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="54"/>
-      <c r="H27" s="23"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="30">
+      <c r="C28" s="49"/>
+      <c r="D28" s="29">
         <v>55</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="54"/>
-      <c r="H28" s="23"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="30">
+      <c r="C29" s="49"/>
+      <c r="D29" s="29">
         <v>70</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="54"/>
-      <c r="H29" s="23"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="30">
+      <c r="C30" s="50"/>
+      <c r="D30" s="29">
         <v>20</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="24" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="55"/>
-      <c r="H30" s="23"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="29">
         <f>SUM(D22:D30)</f>
         <v>405</v>
       </c>
-      <c r="E31" s="25"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="14"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="24"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="23"/>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="49">
+      <c r="C32" s="48">
         <v>43595</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="29">
         <v>20</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="23"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="30">
-        <v>45</v>
-      </c>
-      <c r="E33" s="25" t="s">
+      <c r="C33" s="49"/>
+      <c r="D33" s="29">
+        <v>45</v>
+      </c>
+      <c r="E33" s="24" t="s">
         <v>55</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="54"/>
-      <c r="H33" s="23"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="22"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="30">
+      <c r="C34" s="49"/>
+      <c r="D34" s="29">
         <v>70</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="23"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="30">
+      <c r="C35" s="49"/>
+      <c r="D35" s="29">
         <v>90</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="54"/>
-      <c r="H35" s="23"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="22"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="30">
-        <v>45</v>
-      </c>
-      <c r="E36" s="25" t="s">
+      <c r="C36" s="49"/>
+      <c r="D36" s="29">
+        <v>45</v>
+      </c>
+      <c r="E36" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="54"/>
-      <c r="H36" s="23"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="30">
+      <c r="C37" s="49"/>
+      <c r="D37" s="29">
         <v>20</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="24" t="s">
         <v>61</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="54"/>
-      <c r="H37" s="23"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="30">
+      <c r="C38" s="50"/>
+      <c r="D38" s="29">
         <v>25</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="24" t="s">
         <v>63</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="55"/>
-      <c r="H38" s="23"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="22"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="29">
         <f>SUM(D32:D38)</f>
         <v>315</v>
       </c>
-      <c r="E39" s="25"/>
+      <c r="E39" s="24"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="24"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="23"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="49">
+      <c r="C40" s="48">
         <v>43599</v>
       </c>
-      <c r="D40" s="30">
+      <c r="D40" s="29">
         <v>30</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="27" t="s">
         <v>68</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="23"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="30">
+      <c r="C41" s="49"/>
+      <c r="D41" s="29">
         <v>15</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="24" t="s">
         <v>69</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="54"/>
-      <c r="H41" s="23"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="30">
-        <v>45</v>
-      </c>
-      <c r="E42" s="25" t="s">
+      <c r="C42" s="49"/>
+      <c r="D42" s="29">
+        <v>45</v>
+      </c>
+      <c r="E42" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="54"/>
-      <c r="H42" s="23"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="30">
-        <v>45</v>
-      </c>
-      <c r="E43" s="25" t="s">
+      <c r="C43" s="49"/>
+      <c r="D43" s="29">
+        <v>45</v>
+      </c>
+      <c r="E43" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="54"/>
-      <c r="H43" s="23"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="22"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="30">
-        <v>45</v>
-      </c>
-      <c r="E44" s="25" t="s">
+      <c r="C44" s="49"/>
+      <c r="D44" s="29">
+        <v>45</v>
+      </c>
+      <c r="E44" s="24" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="54"/>
-      <c r="H44" s="23"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="22"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="30">
-        <v>45</v>
-      </c>
-      <c r="E45" s="25" t="s">
+      <c r="C45" s="49"/>
+      <c r="D45" s="29">
+        <v>45</v>
+      </c>
+      <c r="E45" s="24" t="s">
         <v>75</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="54"/>
-      <c r="H45" s="23"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="30">
-        <v>45</v>
-      </c>
-      <c r="E46" s="25" t="s">
+      <c r="C46" s="49"/>
+      <c r="D46" s="29">
+        <v>45</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>75</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="54"/>
-      <c r="H46" s="23"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="22"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="30">
-        <v>45</v>
-      </c>
-      <c r="E47" s="25" t="s">
+      <c r="C47" s="49"/>
+      <c r="D47" s="29">
+        <v>45</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="54"/>
-      <c r="H47" s="23"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="22"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="30">
+      <c r="C48" s="49"/>
+      <c r="D48" s="29">
         <v>15</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="24" t="s">
         <v>78</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="54"/>
-      <c r="H48" s="23"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="22"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="30">
+      <c r="C49" s="49"/>
+      <c r="D49" s="29">
         <v>30</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="E49" s="24" t="s">
         <v>83</v>
       </c>
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="54"/>
-      <c r="H49" s="23"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="22"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="30">
-        <v>45</v>
-      </c>
-      <c r="E50" s="25" t="s">
+      <c r="C50" s="50"/>
+      <c r="D50" s="29">
+        <v>45</v>
+      </c>
+      <c r="E50" s="24" t="s">
         <v>85</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="55"/>
-      <c r="H50" s="23"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="22"/>
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="4"/>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="29">
         <f>SUM(D40:D50)</f>
         <v>405</v>
       </c>
-      <c r="E51" s="25"/>
+      <c r="E51" s="24"/>
       <c r="F51" s="14"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="24"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="23"/>
       <c r="I51" s="5"/>
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="49">
+      <c r="C52" s="48">
         <v>43600</v>
       </c>
-      <c r="D52" s="30">
+      <c r="D52" s="29">
         <v>60</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="E52" s="24" t="s">
         <v>88</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="59" t="s">
+      <c r="G52" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="H52" s="23"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="30">
+      <c r="C53" s="49"/>
+      <c r="D53" s="29">
         <v>60</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="24" t="s">
         <v>90</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="60"/>
-      <c r="H53" s="23"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="30">
-        <v>45</v>
-      </c>
-      <c r="E54" s="25" t="s">
+      <c r="C54" s="49"/>
+      <c r="D54" s="29">
+        <v>45</v>
+      </c>
+      <c r="E54" s="24" t="s">
         <v>83</v>
       </c>
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="60"/>
-      <c r="H54" s="23"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="30">
+      <c r="C55" s="49"/>
+      <c r="D55" s="29">
         <v>15</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="60"/>
-      <c r="H55" s="23"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="30">
-        <v>45</v>
-      </c>
-      <c r="E56" s="25" t="s">
+      <c r="C56" s="50"/>
+      <c r="D56" s="29">
+        <v>45</v>
+      </c>
+      <c r="E56" s="24" t="s">
         <v>85</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="61"/>
-      <c r="H56" s="23"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D57" s="30">
+      <c r="D57" s="29">
         <f>SUM(D52:D56)</f>
         <v>225</v>
       </c>
-      <c r="E57" s="25"/>
+      <c r="E57" s="24"/>
       <c r="F57" s="14"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="24"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="23"/>
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="49">
+      <c r="C58" s="48">
         <v>43601</v>
       </c>
-      <c r="D58" s="30">
+      <c r="D58" s="29">
         <v>30</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="E58" s="24" t="s">
         <v>98</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="56" t="s">
+      <c r="G58" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="H58" s="23"/>
+      <c r="H58" s="22"/>
       <c r="I58" s="5"/>
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="30">
+      <c r="C59" s="49"/>
+      <c r="D59" s="29">
         <v>15</v>
       </c>
-      <c r="E59" s="25" t="s">
+      <c r="E59" s="24" t="s">
         <v>99</v>
       </c>
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="54"/>
-      <c r="H59" s="23"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="22"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="30">
-        <v>45</v>
-      </c>
-      <c r="E60" s="25" t="s">
+      <c r="C60" s="49"/>
+      <c r="D60" s="29">
+        <v>45</v>
+      </c>
+      <c r="E60" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="54"/>
-      <c r="H60" s="23"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="22"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="30">
+      <c r="C61" s="49"/>
+      <c r="D61" s="29">
         <v>90</v>
       </c>
-      <c r="E61" s="25" t="s">
+      <c r="E61" s="24" t="s">
         <v>103</v>
       </c>
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="54"/>
-      <c r="H61" s="23"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="22"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="44">
+      <c r="C62" s="49"/>
+      <c r="D62" s="43">
         <v>30</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="E62" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F62" s="46" t="s">
+      <c r="F62" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="54"/>
-      <c r="H62" s="48"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="47"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="30">
+      <c r="C63" s="49"/>
+      <c r="D63" s="29">
         <v>15</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="E63" s="24" t="s">
         <v>85</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="54"/>
-      <c r="H63" s="23"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="22"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="30">
-        <v>45</v>
-      </c>
-      <c r="E64" s="25" t="s">
+      <c r="C64" s="49"/>
+      <c r="D64" s="29">
+        <v>45</v>
+      </c>
+      <c r="E64" s="24" t="s">
         <v>85</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="54"/>
-      <c r="H64" s="23"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="22"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="30">
-        <v>45</v>
-      </c>
-      <c r="E65" s="25" t="s">
+      <c r="C65" s="49"/>
+      <c r="D65" s="29">
+        <v>45</v>
+      </c>
+      <c r="E65" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="54"/>
-      <c r="H65" s="23"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="22"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="30">
+      <c r="C66" s="50"/>
+      <c r="D66" s="29">
         <v>90</v>
       </c>
-      <c r="E66" s="25" t="s">
+      <c r="E66" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="55"/>
-      <c r="H66" s="23"/>
+      <c r="G66" s="53"/>
+      <c r="H66" s="22"/>
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="4"/>
-      <c r="C67" s="21" t="s">
+      <c r="C67" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D67" s="44">
+      <c r="D67" s="43">
         <f>SUM(D58:D66)</f>
         <v>405</v>
       </c>
-      <c r="E67" s="45"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="47"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="46"/>
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="49">
+      <c r="C68" s="48">
         <v>43602</v>
       </c>
-      <c r="D68" s="30">
-        <v>45</v>
-      </c>
-      <c r="E68" s="25" t="s">
+      <c r="D68" s="29">
+        <v>45</v>
+      </c>
+      <c r="E68" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="56" t="s">
+      <c r="G68" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="H68" s="23"/>
+      <c r="H68" s="22"/>
       <c r="I68" s="5"/>
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="30">
-        <v>45</v>
-      </c>
-      <c r="E69" s="25" t="s">
+      <c r="C69" s="49"/>
+      <c r="D69" s="29">
+        <v>45</v>
+      </c>
+      <c r="E69" s="24" t="s">
         <v>113</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="54"/>
-      <c r="H69" s="23"/>
+      <c r="G69" s="52"/>
+      <c r="H69" s="22"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="30">
-        <v>45</v>
-      </c>
-      <c r="E70" s="25" t="s">
+      <c r="C70" s="49"/>
+      <c r="D70" s="29">
+        <v>45</v>
+      </c>
+      <c r="E70" s="24" t="s">
         <v>115</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="54"/>
-      <c r="H70" s="23"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="22"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="30">
-        <v>45</v>
-      </c>
-      <c r="E71" s="45" t="s">
+      <c r="C71" s="49"/>
+      <c r="D71" s="29">
+        <v>45</v>
+      </c>
+      <c r="E71" s="44" t="s">
         <v>71</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="54"/>
-      <c r="H71" s="23"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="22"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="44">
-        <v>45</v>
-      </c>
-      <c r="E72" s="45" t="s">
+      <c r="C72" s="49"/>
+      <c r="D72" s="43">
+        <v>45</v>
+      </c>
+      <c r="E72" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F72" s="46" t="s">
+      <c r="F72" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="54"/>
-      <c r="H72" s="48"/>
+      <c r="G72" s="52"/>
+      <c r="H72" s="47"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="30">
+      <c r="C73" s="50"/>
+      <c r="D73" s="29">
         <v>90</v>
       </c>
-      <c r="E73" s="25" t="s">
+      <c r="E73" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="55"/>
-      <c r="H73" s="23"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="22"/>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D74" s="30">
+      <c r="D74" s="29">
         <f>SUM(D68:D73)</f>
         <v>315</v>
       </c>
-      <c r="E74" s="25"/>
+      <c r="E74" s="24"/>
       <c r="F74" s="14"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="24"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="23"/>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="49">
+      <c r="C75" s="48">
         <v>43606</v>
       </c>
-      <c r="D75" s="30">
-        <v>45</v>
-      </c>
-      <c r="E75" s="25" t="s">
+      <c r="D75" s="29">
+        <v>45</v>
+      </c>
+      <c r="E75" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G75" s="56" t="s">
+      <c r="G75" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="23"/>
+      <c r="H75" s="22"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="44">
+      <c r="C76" s="49"/>
+      <c r="D76" s="43">
         <v>90</v>
       </c>
-      <c r="E76" s="25" t="s">
+      <c r="E76" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F76" s="46" t="s">
+      <c r="F76" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="54"/>
-      <c r="H76" s="48"/>
+      <c r="G76" s="52"/>
+      <c r="H76" s="47"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="30">
-        <v>45</v>
-      </c>
-      <c r="E77" s="25" t="s">
+      <c r="C77" s="49"/>
+      <c r="D77" s="29">
+        <v>45</v>
+      </c>
+      <c r="E77" s="24" t="s">
         <v>128</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="54"/>
-      <c r="H77" s="23"/>
+      <c r="G77" s="52"/>
+      <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="44">
+      <c r="C78" s="49"/>
+      <c r="D78" s="43">
         <v>90</v>
       </c>
-      <c r="E78" s="25" t="s">
+      <c r="E78" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F78" s="46" t="s">
+      <c r="F78" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G78" s="54"/>
-      <c r="H78" s="48"/>
+      <c r="G78" s="52"/>
+      <c r="H78" s="47"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="30">
+      <c r="C79" s="49"/>
+      <c r="D79" s="29">
         <v>90</v>
       </c>
-      <c r="E79" s="25" t="s">
+      <c r="E79" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="54"/>
-      <c r="H79" s="23"/>
+      <c r="G79" s="52"/>
+      <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="51"/>
-      <c r="D80" s="30">
-        <v>45</v>
-      </c>
-      <c r="E80" s="25" t="s">
+      <c r="C80" s="50"/>
+      <c r="D80" s="29">
+        <v>45</v>
+      </c>
+      <c r="E80" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G80" s="55"/>
-      <c r="H80" s="23"/>
+      <c r="G80" s="53"/>
+      <c r="H80" s="22"/>
       <c r="I80" s="5"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D81" s="30">
+      <c r="D81" s="29">
         <f>SUM(D75:D80)</f>
         <v>405</v>
       </c>
-      <c r="E81" s="25"/>
+      <c r="E81" s="24"/>
       <c r="F81" s="14"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="24"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="23"/>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="49">
+      <c r="C82" s="48">
         <v>43607</v>
       </c>
-      <c r="D82" s="30">
-        <v>45</v>
-      </c>
-      <c r="E82" s="25" t="s">
+      <c r="D82" s="29">
+        <v>45</v>
+      </c>
+      <c r="E82" s="24" t="s">
         <v>130</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G82" s="59" t="s">
+      <c r="G82" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="H82" s="23"/>
+      <c r="H82" s="22"/>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="30">
-        <v>45</v>
-      </c>
-      <c r="E83" s="25" t="s">
+      <c r="C83" s="49"/>
+      <c r="D83" s="29">
+        <v>45</v>
+      </c>
+      <c r="E83" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G83" s="60"/>
-      <c r="H83" s="23"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="30">
+      <c r="C84" s="49"/>
+      <c r="D84" s="29">
         <v>90</v>
       </c>
-      <c r="E84" s="25" t="s">
+      <c r="E84" s="24" t="s">
         <v>71</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="60"/>
-      <c r="H84" s="23"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="30">
-        <v>45</v>
-      </c>
-      <c r="E85" s="25" t="s">
+      <c r="C85" s="49"/>
+      <c r="D85" s="29">
+        <v>45</v>
+      </c>
+      <c r="E85" s="24" t="s">
         <v>128</v>
       </c>
       <c r="F85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G85" s="61"/>
-      <c r="H85" s="23"/>
+      <c r="G85" s="56"/>
+      <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="4"/>
-      <c r="C86" s="21" t="s">
+      <c r="C86" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D86" s="30">
+      <c r="D86" s="29">
         <f>SUM(D82:D85)</f>
         <v>225</v>
       </c>
-      <c r="E86" s="25"/>
+      <c r="E86" s="24"/>
       <c r="F86" s="14"/>
-      <c r="G86" s="30"/>
-      <c r="H86" s="24"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="23"/>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B87" s="4"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="30"/>
-      <c r="H87" s="24"/>
+      <c r="C87" s="48">
+        <v>43608</v>
+      </c>
+      <c r="D87" s="29">
+        <v>45</v>
+      </c>
+      <c r="E87" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G87" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="H87" s="22"/>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B88" s="8"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="9"/>
-    </row>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B88" s="4"/>
+      <c r="C88" s="49"/>
+      <c r="D88" s="29">
+        <v>70</v>
+      </c>
+      <c r="E88" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G88" s="52"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B89" s="4"/>
+      <c r="C89" s="49"/>
+      <c r="D89" s="29">
+        <v>55</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="G89" s="52"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B90" s="4"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="29">
+        <v>55</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G90" s="52"/>
+      <c r="H90" s="22"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B91" s="4"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="29">
+        <v>90</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="52"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B92" s="4"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="29">
+        <v>45</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="G92" s="52"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B93" s="4"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="29">
+        <v>45</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="G93" s="53"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="4"/>
+      <c r="C94" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D94" s="29">
+        <f>SUM(D87:D93)</f>
+        <v>405</v>
+      </c>
+      <c r="E94" s="24"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="B95" s="4"/>
+      <c r="C95" s="48">
+        <v>43609</v>
+      </c>
+      <c r="D95" s="29">
+        <v>30</v>
+      </c>
+      <c r="E95" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G95" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="H95" s="22"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B96" s="4"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="29">
+        <v>15</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G96" s="52"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="B97" s="4"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="29">
+        <v>45</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G97" s="52"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B98" s="4"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="29">
+        <v>45</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G98" s="52"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B99" s="4"/>
+      <c r="C99" s="49"/>
+      <c r="D99" s="29">
+        <v>90</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G99" s="52"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B100" s="4"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="29">
+        <v>45</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G100" s="52"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="4"/>
+      <c r="C101" s="49"/>
+      <c r="D101" s="29">
+        <v>20</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G101" s="52"/>
+      <c r="H101" s="22"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B102" s="4"/>
+      <c r="C102" s="50"/>
+      <c r="D102" s="29">
+        <v>25</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G102" s="53"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B103" s="4"/>
+      <c r="C103" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D103" s="29">
+        <f>SUM(D95:D102)</f>
+        <v>315</v>
+      </c>
+      <c r="E103" s="24"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="23"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B104" s="8"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="35"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="9"/>
+    </row>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="G68:G73"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="G75:G80"/>
-    <mergeCell ref="G82:G85"/>
-    <mergeCell ref="C75:C80"/>
+  <mergeCells count="27">
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="G95:G102"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -2829,12 +3153,17 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="G75:G80"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="C75:C80"/>
     <mergeCell ref="C68:C73"/>
+    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="G87:G93"/>
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Affichage d'un element si un jour contient une tâche ou un rdv + divers réglages
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
     <t>Activités</t>
   </si>
@@ -498,6 +498,42 @@
   </si>
   <si>
     <t xml:space="preserve">Bonne avancée avec la mise en place de la validation de compte par mail. </t>
+  </si>
+  <si>
+    <t>Affichage des tâche et rendez-vous qui sont trop longue (descripition ou commentaire trop long) et ordonner mes tâches et rendez-vous sur mes requêtes</t>
+  </si>
+  <si>
+    <t>Affichage uniquement des tâches et rendez-vous à venir dans la partie Mes tâches et rendez-vous, paramétrage réglage dynamique de certains éléments du formulaire</t>
+  </si>
+  <si>
+    <t>Divers modifications de la dernière review avec ma chef de projet, réglage de quelques textes qui n'allait pas et certains affichage un peu limite.</t>
+  </si>
+  <si>
+    <t>Affichage d'un élément sur le calendrier pour les jours qui contiennent des tâches ou des rendez-vous dans la journée</t>
+  </si>
+  <si>
+    <t>Revue de mes pattern sur mes différents formulaire + validation d'inscription par mail quelques modifications</t>
+  </si>
+  <si>
+    <t>28.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Bonne avancé du code de mon projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test d'un mail de rappel avec l'heure précise à laquelle le mail doit être envoyer grâce à un script et le planificateur de tâche, </t>
+  </si>
+  <si>
+    <t>Réglage de certains détails de mon code vis-à-vis des différents tests réalisé</t>
+  </si>
+  <si>
+    <t>Création d'un script afin d'indiquer a l'utilisateur qu'il a un rendez-vous ou une tâches dans le jour précis</t>
+  </si>
+  <si>
+    <t>29.05.2019, total durée</t>
+  </si>
+  <si>
+    <t>Petit bloquage sur le mail de rappel pour l'utilisateur avant une tâche ou un rendez-vous</t>
   </si>
 </sst>
 </file>
@@ -849,7 +885,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -975,6 +1011,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -990,6 +1029,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1007,9 +1049,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1462,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M147"/>
+  <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1483,31 +1522,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="60"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1569,7 +1608,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="59">
+      <c r="C9" s="61">
         <v>43592</v>
       </c>
       <c r="D9" s="39">
@@ -1581,7 +1620,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="60" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1589,7 +1628,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="29">
         <v>75</v>
       </c>
@@ -1599,13 +1638,13 @@
       <c r="F10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="22"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="29">
         <v>45</v>
       </c>
@@ -1615,13 +1654,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="22"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="29">
         <v>75</v>
       </c>
@@ -1631,13 +1670,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="22"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="29">
         <v>15</v>
       </c>
@@ -1647,13 +1686,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="22"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="29">
         <v>30</v>
       </c>
@@ -1663,13 +1702,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="22"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="29">
         <v>75</v>
       </c>
@@ -1679,13 +1718,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="53"/>
       <c r="H15" s="22"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="29">
         <v>30</v>
       </c>
@@ -1695,7 +1734,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="22"/>
       <c r="I16" s="5"/>
     </row>
@@ -1716,7 +1755,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="48">
+      <c r="C18" s="49">
         <v>43593</v>
       </c>
       <c r="D18" s="29">
@@ -1728,7 +1767,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="52" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="22"/>
@@ -1736,7 +1775,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="49"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="29">
         <v>90</v>
       </c>
@@ -1746,13 +1785,13 @@
       <c r="F19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="52"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="22"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="50"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="29">
         <v>45</v>
       </c>
@@ -1762,7 +1801,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="53"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="22"/>
       <c r="I20" s="5"/>
     </row>
@@ -1783,7 +1822,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="48">
+      <c r="C22" s="49">
         <v>43594</v>
       </c>
       <c r="D22" s="29">
@@ -1795,7 +1834,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="51" t="s">
+      <c r="G22" s="52" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="22"/>
@@ -1803,7 +1842,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="29">
         <v>30</v>
       </c>
@@ -1813,13 +1852,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="52"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="22"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="49"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="29">
         <v>70</v>
       </c>
@@ -1829,13 +1868,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="53"/>
       <c r="H24" s="22"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="29">
         <v>35</v>
       </c>
@@ -1845,13 +1884,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="53"/>
       <c r="H25" s="22"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="29">
         <v>20</v>
       </c>
@@ -1861,13 +1900,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="53"/>
       <c r="H26" s="22"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="29">
         <v>45</v>
       </c>
@@ -1877,13 +1916,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="53"/>
       <c r="H27" s="22"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="49"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="29">
         <v>55</v>
       </c>
@@ -1893,13 +1932,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="52"/>
+      <c r="G28" s="53"/>
       <c r="H28" s="22"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="49"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="29">
         <v>70</v>
       </c>
@@ -1909,13 +1948,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="52"/>
+      <c r="G29" s="53"/>
       <c r="H29" s="22"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="50"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="29">
         <v>20</v>
       </c>
@@ -1925,7 +1964,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="53"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="22"/>
       <c r="I30" s="5"/>
     </row>
@@ -1946,7 +1985,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="48">
+      <c r="C32" s="49">
         <v>43595</v>
       </c>
       <c r="D32" s="29">
@@ -1958,7 +1997,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="51" t="s">
+      <c r="G32" s="52" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="22"/>
@@ -1966,7 +2005,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="49"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="29">
         <v>45</v>
       </c>
@@ -1976,13 +2015,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="52"/>
+      <c r="G33" s="53"/>
       <c r="H33" s="22"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="49"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="29">
         <v>70</v>
       </c>
@@ -1992,13 +2031,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="52"/>
+      <c r="G34" s="53"/>
       <c r="H34" s="22"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="49"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="29">
         <v>90</v>
       </c>
@@ -2008,13 +2047,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="52"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="22"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="49"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="29">
         <v>45</v>
       </c>
@@ -2024,13 +2063,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="22"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="49"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="29">
         <v>20</v>
       </c>
@@ -2040,13 +2079,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="52"/>
+      <c r="G37" s="53"/>
       <c r="H37" s="22"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="50"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="29">
         <v>25</v>
       </c>
@@ -2056,7 +2095,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="53"/>
+      <c r="G38" s="54"/>
       <c r="H38" s="22"/>
       <c r="I38" s="5"/>
     </row>
@@ -2077,7 +2116,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="48">
+      <c r="C40" s="49">
         <v>43599</v>
       </c>
       <c r="D40" s="29">
@@ -2089,7 +2128,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="51" t="s">
+      <c r="G40" s="52" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="22"/>
@@ -2097,7 +2136,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="49"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="29">
         <v>15</v>
       </c>
@@ -2107,13 +2146,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="52"/>
+      <c r="G41" s="53"/>
       <c r="H41" s="22"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="49"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="29">
         <v>45</v>
       </c>
@@ -2123,13 +2162,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="53"/>
       <c r="H42" s="22"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="49"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="29">
         <v>45</v>
       </c>
@@ -2139,13 +2178,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="52"/>
+      <c r="G43" s="53"/>
       <c r="H43" s="22"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="29">
         <v>45</v>
       </c>
@@ -2155,13 +2194,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="52"/>
+      <c r="G44" s="53"/>
       <c r="H44" s="22"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="49"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="29">
         <v>45</v>
       </c>
@@ -2171,13 +2210,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="52"/>
+      <c r="G45" s="53"/>
       <c r="H45" s="22"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="49"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="29">
         <v>45</v>
       </c>
@@ -2187,13 +2226,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="52"/>
+      <c r="G46" s="53"/>
       <c r="H46" s="22"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="49"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="29">
         <v>45</v>
       </c>
@@ -2203,13 +2242,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="52"/>
+      <c r="G47" s="53"/>
       <c r="H47" s="22"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="49"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="29">
         <v>15</v>
       </c>
@@ -2219,13 +2258,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="52"/>
+      <c r="G48" s="53"/>
       <c r="H48" s="22"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="49"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="29">
         <v>30</v>
       </c>
@@ -2235,13 +2274,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="52"/>
+      <c r="G49" s="53"/>
       <c r="H49" s="22"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="50"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="29">
         <v>45</v>
       </c>
@@ -2251,7 +2290,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="53"/>
+      <c r="G50" s="54"/>
       <c r="H50" s="22"/>
       <c r="I50" s="5"/>
     </row>
@@ -2272,7 +2311,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="48">
+      <c r="C52" s="49">
         <v>43600</v>
       </c>
       <c r="D52" s="29">
@@ -2284,7 +2323,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="54" t="s">
+      <c r="G52" s="56" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="22"/>
@@ -2292,7 +2331,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="49"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="29">
         <v>60</v>
       </c>
@@ -2302,13 +2341,13 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="55"/>
+      <c r="G53" s="57"/>
       <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="29">
         <v>45</v>
       </c>
@@ -2318,13 +2357,13 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="55"/>
+      <c r="G54" s="57"/>
       <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="29">
         <v>15</v>
       </c>
@@ -2334,13 +2373,13 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="55"/>
+      <c r="G55" s="57"/>
       <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="50"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="29">
         <v>45</v>
       </c>
@@ -2350,7 +2389,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="56"/>
+      <c r="G56" s="58"/>
       <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
@@ -2371,7 +2410,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="48">
+      <c r="C58" s="49">
         <v>43601</v>
       </c>
       <c r="D58" s="29">
@@ -2383,7 +2422,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="51" t="s">
+      <c r="G58" s="52" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="22"/>
@@ -2391,7 +2430,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="29">
         <v>15</v>
       </c>
@@ -2401,13 +2440,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="52"/>
+      <c r="G59" s="53"/>
       <c r="H59" s="22"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="29">
         <v>45</v>
       </c>
@@ -2417,13 +2456,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="52"/>
+      <c r="G60" s="53"/>
       <c r="H60" s="22"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="29">
         <v>90</v>
       </c>
@@ -2433,13 +2472,13 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="52"/>
+      <c r="G61" s="53"/>
       <c r="H61" s="22"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="43">
         <v>30</v>
       </c>
@@ -2449,13 +2488,13 @@
       <c r="F62" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="52"/>
+      <c r="G62" s="53"/>
       <c r="H62" s="47"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="29">
         <v>15</v>
       </c>
@@ -2465,13 +2504,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="52"/>
+      <c r="G63" s="53"/>
       <c r="H63" s="22"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="49"/>
+      <c r="C64" s="50"/>
       <c r="D64" s="29">
         <v>45</v>
       </c>
@@ -2481,13 +2520,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="52"/>
+      <c r="G64" s="53"/>
       <c r="H64" s="22"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="49"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="29">
         <v>45</v>
       </c>
@@ -2497,13 +2536,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="52"/>
+      <c r="G65" s="53"/>
       <c r="H65" s="22"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="50"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="29">
         <v>90</v>
       </c>
@@ -2513,7 +2552,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="53"/>
+      <c r="G66" s="54"/>
       <c r="H66" s="22"/>
       <c r="I66" s="5"/>
     </row>
@@ -2534,7 +2573,7 @@
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="48">
+      <c r="C68" s="49">
         <v>43602</v>
       </c>
       <c r="D68" s="29">
@@ -2546,7 +2585,7 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="51" t="s">
+      <c r="G68" s="52" t="s">
         <v>120</v>
       </c>
       <c r="H68" s="22"/>
@@ -2554,7 +2593,7 @@
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="49"/>
+      <c r="C69" s="50"/>
       <c r="D69" s="29">
         <v>45</v>
       </c>
@@ -2564,13 +2603,13 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="52"/>
+      <c r="G69" s="53"/>
       <c r="H69" s="22"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="49"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="29">
         <v>45</v>
       </c>
@@ -2580,13 +2619,13 @@
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="52"/>
+      <c r="G70" s="53"/>
       <c r="H70" s="22"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="49"/>
+      <c r="C71" s="50"/>
       <c r="D71" s="29">
         <v>45</v>
       </c>
@@ -2596,13 +2635,13 @@
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="52"/>
+      <c r="G71" s="53"/>
       <c r="H71" s="22"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="49"/>
+      <c r="C72" s="50"/>
       <c r="D72" s="43">
         <v>45</v>
       </c>
@@ -2612,13 +2651,13 @@
       <c r="F72" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="52"/>
+      <c r="G72" s="53"/>
       <c r="H72" s="47"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="50"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="29">
         <v>90</v>
       </c>
@@ -2628,7 +2667,7 @@
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="53"/>
+      <c r="G73" s="54"/>
       <c r="H73" s="22"/>
       <c r="I73" s="5"/>
     </row>
@@ -2649,7 +2688,7 @@
     </row>
     <row r="75" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="48">
+      <c r="C75" s="49">
         <v>43606</v>
       </c>
       <c r="D75" s="29">
@@ -2661,7 +2700,7 @@
       <c r="F75" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G75" s="51" t="s">
+      <c r="G75" s="52" t="s">
         <v>136</v>
       </c>
       <c r="H75" s="22"/>
@@ -2669,7 +2708,7 @@
     </row>
     <row r="76" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="49"/>
+      <c r="C76" s="50"/>
       <c r="D76" s="43">
         <v>90</v>
       </c>
@@ -2679,13 +2718,13 @@
       <c r="F76" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="52"/>
+      <c r="G76" s="53"/>
       <c r="H76" s="47"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="49"/>
+      <c r="C77" s="50"/>
       <c r="D77" s="29">
         <v>45</v>
       </c>
@@ -2695,13 +2734,13 @@
       <c r="F77" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="52"/>
+      <c r="G77" s="53"/>
       <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="49"/>
+      <c r="C78" s="50"/>
       <c r="D78" s="43">
         <v>90</v>
       </c>
@@ -2711,13 +2750,13 @@
       <c r="F78" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G78" s="52"/>
+      <c r="G78" s="53"/>
       <c r="H78" s="47"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="49"/>
+      <c r="C79" s="50"/>
       <c r="D79" s="29">
         <v>90</v>
       </c>
@@ -2727,13 +2766,13 @@
       <c r="F79" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="52"/>
+      <c r="G79" s="53"/>
       <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="50"/>
+      <c r="C80" s="51"/>
       <c r="D80" s="29">
         <v>45</v>
       </c>
@@ -2743,7 +2782,7 @@
       <c r="F80" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G80" s="53"/>
+      <c r="G80" s="54"/>
       <c r="H80" s="22"/>
       <c r="I80" s="5"/>
     </row>
@@ -2764,7 +2803,7 @@
     </row>
     <row r="82" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="48">
+      <c r="C82" s="49">
         <v>43607</v>
       </c>
       <c r="D82" s="29">
@@ -2776,7 +2815,7 @@
       <c r="F82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G82" s="54" t="s">
+      <c r="G82" s="56" t="s">
         <v>137</v>
       </c>
       <c r="H82" s="22"/>
@@ -2784,7 +2823,7 @@
     </row>
     <row r="83" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="49"/>
+      <c r="C83" s="50"/>
       <c r="D83" s="29">
         <v>45</v>
       </c>
@@ -2794,13 +2833,13 @@
       <c r="F83" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G83" s="55"/>
+      <c r="G83" s="57"/>
       <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
-      <c r="C84" s="49"/>
+      <c r="C84" s="50"/>
       <c r="D84" s="29">
         <v>90</v>
       </c>
@@ -2810,13 +2849,13 @@
       <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="55"/>
+      <c r="G84" s="57"/>
       <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
-      <c r="C85" s="49"/>
+      <c r="C85" s="50"/>
       <c r="D85" s="29">
         <v>45</v>
       </c>
@@ -2826,7 +2865,7 @@
       <c r="F85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G85" s="56"/>
+      <c r="G85" s="58"/>
       <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
@@ -2847,7 +2886,7 @@
     </row>
     <row r="87" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B87" s="4"/>
-      <c r="C87" s="48">
+      <c r="C87" s="49">
         <v>43608</v>
       </c>
       <c r="D87" s="29">
@@ -2859,7 +2898,7 @@
       <c r="F87" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G87" s="51" t="s">
+      <c r="G87" s="52" t="s">
         <v>146</v>
       </c>
       <c r="H87" s="22"/>
@@ -2867,7 +2906,7 @@
     </row>
     <row r="88" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B88" s="4"/>
-      <c r="C88" s="49"/>
+      <c r="C88" s="50"/>
       <c r="D88" s="29">
         <v>70</v>
       </c>
@@ -2877,13 +2916,13 @@
       <c r="F88" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G88" s="52"/>
+      <c r="G88" s="53"/>
       <c r="H88" s="22"/>
       <c r="I88" s="5"/>
     </row>
     <row r="89" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B89" s="4"/>
-      <c r="C89" s="49"/>
+      <c r="C89" s="50"/>
       <c r="D89" s="29">
         <v>55</v>
       </c>
@@ -2893,13 +2932,13 @@
       <c r="F89" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="G89" s="52"/>
+      <c r="G89" s="53"/>
       <c r="H89" s="22"/>
       <c r="I89" s="5"/>
     </row>
     <row r="90" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B90" s="4"/>
-      <c r="C90" s="49"/>
+      <c r="C90" s="50"/>
       <c r="D90" s="29">
         <v>55</v>
       </c>
@@ -2909,13 +2948,13 @@
       <c r="F90" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="52"/>
+      <c r="G90" s="53"/>
       <c r="H90" s="22"/>
       <c r="I90" s="5"/>
     </row>
     <row r="91" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B91" s="4"/>
-      <c r="C91" s="49"/>
+      <c r="C91" s="50"/>
       <c r="D91" s="29">
         <v>90</v>
       </c>
@@ -2925,13 +2964,13 @@
       <c r="F91" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G91" s="52"/>
+      <c r="G91" s="53"/>
       <c r="H91" s="22"/>
       <c r="I91" s="5"/>
     </row>
     <row r="92" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
-      <c r="C92" s="49"/>
+      <c r="C92" s="50"/>
       <c r="D92" s="29">
         <v>45</v>
       </c>
@@ -2941,13 +2980,13 @@
       <c r="F92" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G92" s="52"/>
+      <c r="G92" s="53"/>
       <c r="H92" s="22"/>
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B93" s="4"/>
-      <c r="C93" s="50"/>
+      <c r="C93" s="51"/>
       <c r="D93" s="29">
         <v>45</v>
       </c>
@@ -2957,7 +2996,7 @@
       <c r="F93" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="G93" s="53"/>
+      <c r="G93" s="54"/>
       <c r="H93" s="22"/>
       <c r="I93" s="5"/>
     </row>
@@ -2978,7 +3017,7 @@
     </row>
     <row r="95" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B95" s="4"/>
-      <c r="C95" s="48">
+      <c r="C95" s="49">
         <v>43609</v>
       </c>
       <c r="D95" s="29">
@@ -2990,7 +3029,7 @@
       <c r="F95" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="G95" s="51" t="s">
+      <c r="G95" s="52" t="s">
         <v>157</v>
       </c>
       <c r="H95" s="22"/>
@@ -2998,7 +3037,7 @@
     </row>
     <row r="96" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B96" s="4"/>
-      <c r="C96" s="49"/>
+      <c r="C96" s="50"/>
       <c r="D96" s="29">
         <v>15</v>
       </c>
@@ -3008,13 +3047,13 @@
       <c r="F96" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G96" s="52"/>
+      <c r="G96" s="53"/>
       <c r="H96" s="22"/>
       <c r="I96" s="5"/>
     </row>
     <row r="97" spans="2:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B97" s="4"/>
-      <c r="C97" s="49"/>
+      <c r="C97" s="50"/>
       <c r="D97" s="29">
         <v>45</v>
       </c>
@@ -3024,13 +3063,13 @@
       <c r="F97" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G97" s="52"/>
+      <c r="G97" s="53"/>
       <c r="H97" s="22"/>
       <c r="I97" s="5"/>
     </row>
     <row r="98" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B98" s="4"/>
-      <c r="C98" s="49"/>
+      <c r="C98" s="50"/>
       <c r="D98" s="29">
         <v>45</v>
       </c>
@@ -3040,13 +3079,13 @@
       <c r="F98" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G98" s="52"/>
+      <c r="G98" s="53"/>
       <c r="H98" s="22"/>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B99" s="4"/>
-      <c r="C99" s="49"/>
+      <c r="C99" s="50"/>
       <c r="D99" s="29">
         <v>90</v>
       </c>
@@ -3056,13 +3095,13 @@
       <c r="F99" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G99" s="52"/>
+      <c r="G99" s="53"/>
       <c r="H99" s="22"/>
       <c r="I99" s="5"/>
     </row>
     <row r="100" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B100" s="4"/>
-      <c r="C100" s="49"/>
+      <c r="C100" s="50"/>
       <c r="D100" s="29">
         <v>45</v>
       </c>
@@ -3072,13 +3111,13 @@
       <c r="F100" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="G100" s="52"/>
+      <c r="G100" s="53"/>
       <c r="H100" s="22"/>
       <c r="I100" s="5"/>
     </row>
     <row r="101" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="4"/>
-      <c r="C101" s="49"/>
+      <c r="C101" s="50"/>
       <c r="D101" s="29">
         <v>20</v>
       </c>
@@ -3088,13 +3127,13 @@
       <c r="F101" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G101" s="52"/>
+      <c r="G101" s="53"/>
       <c r="H101" s="22"/>
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B102" s="4"/>
-      <c r="C102" s="50"/>
+      <c r="C102" s="51"/>
       <c r="D102" s="29">
         <v>25</v>
       </c>
@@ -3104,7 +3143,7 @@
       <c r="F102" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G102" s="53"/>
+      <c r="G102" s="54"/>
       <c r="H102" s="22"/>
       <c r="I102" s="5"/>
     </row>
@@ -3123,27 +3162,202 @@
       <c r="H103" s="23"/>
       <c r="I103" s="5"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B104" s="8"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="35"/>
-      <c r="H104" s="19"/>
-      <c r="I104" s="9"/>
-    </row>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" spans="2:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="B104" s="4"/>
+      <c r="C104" s="49">
+        <v>43613</v>
+      </c>
+      <c r="D104" s="43">
+        <v>90</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F104" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="G104" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H104" s="47"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="B105" s="4"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="43">
+        <v>90</v>
+      </c>
+      <c r="E105" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F105" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="G105" s="53"/>
+      <c r="H105" s="47"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B106" s="4"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="43">
+        <v>45</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F106" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="G106" s="53"/>
+      <c r="H106" s="47"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B107" s="4"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="43">
+        <v>90</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F107" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="G107" s="53"/>
+      <c r="H107" s="47"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B108" s="4"/>
+      <c r="C108" s="51"/>
+      <c r="D108" s="43">
+        <v>90</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F108" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="G108" s="54"/>
+      <c r="H108" s="47"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B109" s="4"/>
+      <c r="C109" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D109" s="43">
+        <f>SUM(D104:D108)</f>
+        <v>405</v>
+      </c>
+      <c r="E109" s="44"/>
+      <c r="F109" s="45"/>
+      <c r="G109" s="43"/>
+      <c r="H109" s="46"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B110" s="4"/>
+      <c r="C110" s="49">
+        <v>43614</v>
+      </c>
+      <c r="D110" s="43">
+        <v>90</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F110" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="G110" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="H110" s="47"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B111" s="4"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="43">
+        <v>90</v>
+      </c>
+      <c r="E111" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F111" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="G111" s="57"/>
+      <c r="H111" s="47"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B112" s="4"/>
+      <c r="C112" s="51"/>
+      <c r="D112" s="43">
+        <v>45</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F112" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="G112" s="58"/>
+      <c r="H112" s="47"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B113" s="4"/>
+      <c r="C113" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D113" s="43">
+        <f>SUM(D110:D112)</f>
+        <v>225</v>
+      </c>
+      <c r="E113" s="44"/>
+      <c r="F113" s="45"/>
+      <c r="G113" s="43"/>
+      <c r="H113" s="46"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" s="4"/>
+      <c r="C114" s="48"/>
+      <c r="D114" s="43"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="45"/>
+      <c r="G114" s="43"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B115" s="8"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="35"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="35"/>
+      <c r="H115" s="19"/>
+      <c r="I115" s="9"/>
+    </row>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C95:C102"/>
-    <mergeCell ref="G95:G102"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
+  <mergeCells count="31">
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C104:C108"/>
+    <mergeCell ref="G104:G108"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="G110:G112"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -3153,6 +3367,13 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="G95:G102"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
     <mergeCell ref="C52:C56"/>
     <mergeCell ref="C82:C85"/>
     <mergeCell ref="G75:G80"/>
@@ -3162,8 +3383,6 @@
     <mergeCell ref="C87:C93"/>
     <mergeCell ref="G87:G93"/>
     <mergeCell ref="G68:G73"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Code final partie 1
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="171">
   <si>
     <t>Activités</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>Petit bloquage sur le mail de rappel pour l'utilisateur avant une tâche ou un rendez-vous</t>
+  </si>
+  <si>
+    <t>Diego Sanchez et Frédérique Andolfatto, Code</t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1014,6 +1017,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1029,26 +1035,26 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1501,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M158"/>
+  <dimension ref="A1:M173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1539,14 +1545,14 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="55"/>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1628,7 +1634,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="29">
         <v>75</v>
       </c>
@@ -1638,13 +1644,13 @@
       <c r="F10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="53"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="22"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="29">
         <v>45</v>
       </c>
@@ -1654,13 +1660,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="53"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="22"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="29">
         <v>75</v>
       </c>
@@ -1670,13 +1676,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="22"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="29">
         <v>15</v>
       </c>
@@ -1686,13 +1692,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="53"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="22"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="29">
         <v>30</v>
       </c>
@@ -1702,13 +1708,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="22"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="29">
         <v>75</v>
       </c>
@@ -1718,13 +1724,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="22"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="29">
         <v>30</v>
       </c>
@@ -1734,7 +1740,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="22"/>
       <c r="I16" s="5"/>
     </row>
@@ -1755,7 +1761,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="49">
+      <c r="C18" s="50">
         <v>43593</v>
       </c>
       <c r="D18" s="29">
@@ -1767,7 +1773,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="53" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="22"/>
@@ -1775,7 +1781,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="29">
         <v>90</v>
       </c>
@@ -1785,13 +1791,13 @@
       <c r="F19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="22"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="51"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="29">
         <v>45</v>
       </c>
@@ -1801,7 +1807,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="22"/>
       <c r="I20" s="5"/>
     </row>
@@ -1822,7 +1828,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="49">
+      <c r="C22" s="50">
         <v>43594</v>
       </c>
       <c r="D22" s="29">
@@ -1834,7 +1840,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="53" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="22"/>
@@ -1842,7 +1848,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="50"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="29">
         <v>30</v>
       </c>
@@ -1852,13 +1858,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="53"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="22"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="50"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="29">
         <v>70</v>
       </c>
@@ -1868,13 +1874,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="53"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="22"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="29">
         <v>35</v>
       </c>
@@ -1884,13 +1890,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="53"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="22"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="29">
         <v>20</v>
       </c>
@@ -1900,13 +1906,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="53"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="22"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="29">
         <v>45</v>
       </c>
@@ -1916,13 +1922,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="53"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="22"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="50"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="29">
         <v>55</v>
       </c>
@@ -1932,13 +1938,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="53"/>
+      <c r="G28" s="54"/>
       <c r="H28" s="22"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="50"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="29">
         <v>70</v>
       </c>
@@ -1948,13 +1954,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="53"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="22"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="51"/>
+      <c r="C30" s="52"/>
       <c r="D30" s="29">
         <v>20</v>
       </c>
@@ -1964,7 +1970,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="55"/>
       <c r="H30" s="22"/>
       <c r="I30" s="5"/>
     </row>
@@ -1985,7 +1991,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="49">
+      <c r="C32" s="50">
         <v>43595</v>
       </c>
       <c r="D32" s="29">
@@ -1997,7 +2003,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="52" t="s">
+      <c r="G32" s="53" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="22"/>
@@ -2005,7 +2011,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="50"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="29">
         <v>45</v>
       </c>
@@ -2015,13 +2021,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="53"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="22"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="50"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="29">
         <v>70</v>
       </c>
@@ -2031,13 +2037,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="53"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="22"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="50"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="29">
         <v>90</v>
       </c>
@@ -2047,13 +2053,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="53"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="22"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="50"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="29">
         <v>45</v>
       </c>
@@ -2063,13 +2069,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="53"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="22"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="50"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="29">
         <v>20</v>
       </c>
@@ -2079,13 +2085,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="53"/>
+      <c r="G37" s="54"/>
       <c r="H37" s="22"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="51"/>
+      <c r="C38" s="52"/>
       <c r="D38" s="29">
         <v>25</v>
       </c>
@@ -2095,7 +2101,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="54"/>
+      <c r="G38" s="55"/>
       <c r="H38" s="22"/>
       <c r="I38" s="5"/>
     </row>
@@ -2116,7 +2122,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="49">
+      <c r="C40" s="50">
         <v>43599</v>
       </c>
       <c r="D40" s="29">
@@ -2128,7 +2134,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="52" t="s">
+      <c r="G40" s="53" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="22"/>
@@ -2136,7 +2142,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="50"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="29">
         <v>15</v>
       </c>
@@ -2146,13 +2152,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="53"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="22"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="50"/>
+      <c r="C42" s="51"/>
       <c r="D42" s="29">
         <v>45</v>
       </c>
@@ -2162,13 +2168,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="53"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="22"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="50"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="29">
         <v>45</v>
       </c>
@@ -2178,13 +2184,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="22"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="50"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="29">
         <v>45</v>
       </c>
@@ -2194,13 +2200,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="53"/>
+      <c r="G44" s="54"/>
       <c r="H44" s="22"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="50"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="29">
         <v>45</v>
       </c>
@@ -2210,13 +2216,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="53"/>
+      <c r="G45" s="54"/>
       <c r="H45" s="22"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="50"/>
+      <c r="C46" s="51"/>
       <c r="D46" s="29">
         <v>45</v>
       </c>
@@ -2226,13 +2232,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="53"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="22"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="50"/>
+      <c r="C47" s="51"/>
       <c r="D47" s="29">
         <v>45</v>
       </c>
@@ -2242,13 +2248,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="53"/>
+      <c r="G47" s="54"/>
       <c r="H47" s="22"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="50"/>
+      <c r="C48" s="51"/>
       <c r="D48" s="29">
         <v>15</v>
       </c>
@@ -2258,13 +2264,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="53"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="22"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="50"/>
+      <c r="C49" s="51"/>
       <c r="D49" s="29">
         <v>30</v>
       </c>
@@ -2274,13 +2280,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="53"/>
+      <c r="G49" s="54"/>
       <c r="H49" s="22"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="51"/>
+      <c r="C50" s="52"/>
       <c r="D50" s="29">
         <v>45</v>
       </c>
@@ -2290,7 +2296,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="54"/>
+      <c r="G50" s="55"/>
       <c r="H50" s="22"/>
       <c r="I50" s="5"/>
     </row>
@@ -2311,7 +2317,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="49">
+      <c r="C52" s="50">
         <v>43600</v>
       </c>
       <c r="D52" s="29">
@@ -2331,7 +2337,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="50"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="29">
         <v>60</v>
       </c>
@@ -2347,7 +2353,7 @@
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="50"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="29">
         <v>45</v>
       </c>
@@ -2363,7 +2369,7 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="50"/>
+      <c r="C55" s="51"/>
       <c r="D55" s="29">
         <v>15</v>
       </c>
@@ -2379,7 +2385,7 @@
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="51"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="29">
         <v>45</v>
       </c>
@@ -2410,7 +2416,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="49">
+      <c r="C58" s="50">
         <v>43601</v>
       </c>
       <c r="D58" s="29">
@@ -2422,7 +2428,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="52" t="s">
+      <c r="G58" s="53" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="22"/>
@@ -2430,7 +2436,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="50"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="29">
         <v>15</v>
       </c>
@@ -2440,13 +2446,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="53"/>
+      <c r="G59" s="54"/>
       <c r="H59" s="22"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="50"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="29">
         <v>45</v>
       </c>
@@ -2456,13 +2462,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="53"/>
+      <c r="G60" s="54"/>
       <c r="H60" s="22"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="50"/>
+      <c r="C61" s="51"/>
       <c r="D61" s="29">
         <v>90</v>
       </c>
@@ -2472,13 +2478,13 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="53"/>
+      <c r="G61" s="54"/>
       <c r="H61" s="22"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="50"/>
+      <c r="C62" s="51"/>
       <c r="D62" s="43">
         <v>30</v>
       </c>
@@ -2488,13 +2494,13 @@
       <c r="F62" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="53"/>
+      <c r="G62" s="54"/>
       <c r="H62" s="47"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="50"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="29">
         <v>15</v>
       </c>
@@ -2504,13 +2510,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="53"/>
+      <c r="G63" s="54"/>
       <c r="H63" s="22"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="50"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="29">
         <v>45</v>
       </c>
@@ -2520,13 +2526,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="53"/>
+      <c r="G64" s="54"/>
       <c r="H64" s="22"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="50"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="29">
         <v>45</v>
       </c>
@@ -2536,13 +2542,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="53"/>
+      <c r="G65" s="54"/>
       <c r="H65" s="22"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="51"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="29">
         <v>90</v>
       </c>
@@ -2552,7 +2558,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="54"/>
+      <c r="G66" s="55"/>
       <c r="H66" s="22"/>
       <c r="I66" s="5"/>
     </row>
@@ -2573,7 +2579,7 @@
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="49">
+      <c r="C68" s="50">
         <v>43602</v>
       </c>
       <c r="D68" s="29">
@@ -2585,7 +2591,7 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="52" t="s">
+      <c r="G68" s="53" t="s">
         <v>120</v>
       </c>
       <c r="H68" s="22"/>
@@ -2593,7 +2599,7 @@
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="50"/>
+      <c r="C69" s="51"/>
       <c r="D69" s="29">
         <v>45</v>
       </c>
@@ -2603,13 +2609,13 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="53"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="22"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="50"/>
+      <c r="C70" s="51"/>
       <c r="D70" s="29">
         <v>45</v>
       </c>
@@ -2619,13 +2625,13 @@
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="53"/>
+      <c r="G70" s="54"/>
       <c r="H70" s="22"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="50"/>
+      <c r="C71" s="51"/>
       <c r="D71" s="29">
         <v>45</v>
       </c>
@@ -2635,13 +2641,13 @@
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="53"/>
+      <c r="G71" s="54"/>
       <c r="H71" s="22"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="50"/>
+      <c r="C72" s="51"/>
       <c r="D72" s="43">
         <v>45</v>
       </c>
@@ -2651,13 +2657,13 @@
       <c r="F72" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="53"/>
+      <c r="G72" s="54"/>
       <c r="H72" s="47"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="51"/>
+      <c r="C73" s="52"/>
       <c r="D73" s="29">
         <v>90</v>
       </c>
@@ -2667,7 +2673,7 @@
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="54"/>
+      <c r="G73" s="55"/>
       <c r="H73" s="22"/>
       <c r="I73" s="5"/>
     </row>
@@ -2688,7 +2694,7 @@
     </row>
     <row r="75" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="49">
+      <c r="C75" s="50">
         <v>43606</v>
       </c>
       <c r="D75" s="29">
@@ -2700,7 +2706,7 @@
       <c r="F75" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G75" s="52" t="s">
+      <c r="G75" s="53" t="s">
         <v>136</v>
       </c>
       <c r="H75" s="22"/>
@@ -2708,7 +2714,7 @@
     </row>
     <row r="76" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="50"/>
+      <c r="C76" s="51"/>
       <c r="D76" s="43">
         <v>90</v>
       </c>
@@ -2718,13 +2724,13 @@
       <c r="F76" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="53"/>
+      <c r="G76" s="54"/>
       <c r="H76" s="47"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="50"/>
+      <c r="C77" s="51"/>
       <c r="D77" s="29">
         <v>45</v>
       </c>
@@ -2734,13 +2740,13 @@
       <c r="F77" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="53"/>
+      <c r="G77" s="54"/>
       <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="50"/>
+      <c r="C78" s="51"/>
       <c r="D78" s="43">
         <v>90</v>
       </c>
@@ -2750,13 +2756,13 @@
       <c r="F78" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G78" s="53"/>
+      <c r="G78" s="54"/>
       <c r="H78" s="47"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="50"/>
+      <c r="C79" s="51"/>
       <c r="D79" s="29">
         <v>90</v>
       </c>
@@ -2766,13 +2772,13 @@
       <c r="F79" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="53"/>
+      <c r="G79" s="54"/>
       <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="51"/>
+      <c r="C80" s="52"/>
       <c r="D80" s="29">
         <v>45</v>
       </c>
@@ -2782,7 +2788,7 @@
       <c r="F80" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G80" s="54"/>
+      <c r="G80" s="55"/>
       <c r="H80" s="22"/>
       <c r="I80" s="5"/>
     </row>
@@ -2803,7 +2809,7 @@
     </row>
     <row r="82" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="49">
+      <c r="C82" s="50">
         <v>43607</v>
       </c>
       <c r="D82" s="29">
@@ -2823,7 +2829,7 @@
     </row>
     <row r="83" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="50"/>
+      <c r="C83" s="51"/>
       <c r="D83" s="29">
         <v>45</v>
       </c>
@@ -2839,7 +2845,7 @@
     </row>
     <row r="84" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
-      <c r="C84" s="50"/>
+      <c r="C84" s="51"/>
       <c r="D84" s="29">
         <v>90</v>
       </c>
@@ -2855,7 +2861,7 @@
     </row>
     <row r="85" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
-      <c r="C85" s="50"/>
+      <c r="C85" s="51"/>
       <c r="D85" s="29">
         <v>45</v>
       </c>
@@ -2886,7 +2892,7 @@
     </row>
     <row r="87" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B87" s="4"/>
-      <c r="C87" s="49">
+      <c r="C87" s="50">
         <v>43608</v>
       </c>
       <c r="D87" s="29">
@@ -2898,7 +2904,7 @@
       <c r="F87" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G87" s="52" t="s">
+      <c r="G87" s="53" t="s">
         <v>146</v>
       </c>
       <c r="H87" s="22"/>
@@ -2906,7 +2912,7 @@
     </row>
     <row r="88" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B88" s="4"/>
-      <c r="C88" s="50"/>
+      <c r="C88" s="51"/>
       <c r="D88" s="29">
         <v>70</v>
       </c>
@@ -2916,13 +2922,13 @@
       <c r="F88" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G88" s="53"/>
+      <c r="G88" s="54"/>
       <c r="H88" s="22"/>
       <c r="I88" s="5"/>
     </row>
     <row r="89" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B89" s="4"/>
-      <c r="C89" s="50"/>
+      <c r="C89" s="51"/>
       <c r="D89" s="29">
         <v>55</v>
       </c>
@@ -2932,13 +2938,13 @@
       <c r="F89" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="G89" s="53"/>
+      <c r="G89" s="54"/>
       <c r="H89" s="22"/>
       <c r="I89" s="5"/>
     </row>
     <row r="90" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B90" s="4"/>
-      <c r="C90" s="50"/>
+      <c r="C90" s="51"/>
       <c r="D90" s="29">
         <v>55</v>
       </c>
@@ -2948,13 +2954,13 @@
       <c r="F90" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="53"/>
+      <c r="G90" s="54"/>
       <c r="H90" s="22"/>
       <c r="I90" s="5"/>
     </row>
     <row r="91" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B91" s="4"/>
-      <c r="C91" s="50"/>
+      <c r="C91" s="51"/>
       <c r="D91" s="29">
         <v>90</v>
       </c>
@@ -2964,13 +2970,13 @@
       <c r="F91" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G91" s="53"/>
+      <c r="G91" s="54"/>
       <c r="H91" s="22"/>
       <c r="I91" s="5"/>
     </row>
     <row r="92" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
-      <c r="C92" s="50"/>
+      <c r="C92" s="51"/>
       <c r="D92" s="29">
         <v>45</v>
       </c>
@@ -2980,13 +2986,13 @@
       <c r="F92" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G92" s="53"/>
+      <c r="G92" s="54"/>
       <c r="H92" s="22"/>
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B93" s="4"/>
-      <c r="C93" s="51"/>
+      <c r="C93" s="52"/>
       <c r="D93" s="29">
         <v>45</v>
       </c>
@@ -2996,7 +3002,7 @@
       <c r="F93" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="G93" s="54"/>
+      <c r="G93" s="55"/>
       <c r="H93" s="22"/>
       <c r="I93" s="5"/>
     </row>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="95" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B95" s="4"/>
-      <c r="C95" s="49">
+      <c r="C95" s="50">
         <v>43609</v>
       </c>
       <c r="D95" s="29">
@@ -3029,7 +3035,7 @@
       <c r="F95" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="G95" s="52" t="s">
+      <c r="G95" s="53" t="s">
         <v>157</v>
       </c>
       <c r="H95" s="22"/>
@@ -3037,7 +3043,7 @@
     </row>
     <row r="96" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B96" s="4"/>
-      <c r="C96" s="50"/>
+      <c r="C96" s="51"/>
       <c r="D96" s="29">
         <v>15</v>
       </c>
@@ -3047,13 +3053,13 @@
       <c r="F96" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G96" s="53"/>
+      <c r="G96" s="54"/>
       <c r="H96" s="22"/>
       <c r="I96" s="5"/>
     </row>
     <row r="97" spans="2:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B97" s="4"/>
-      <c r="C97" s="50"/>
+      <c r="C97" s="51"/>
       <c r="D97" s="29">
         <v>45</v>
       </c>
@@ -3063,13 +3069,13 @@
       <c r="F97" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G97" s="53"/>
+      <c r="G97" s="54"/>
       <c r="H97" s="22"/>
       <c r="I97" s="5"/>
     </row>
     <row r="98" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B98" s="4"/>
-      <c r="C98" s="50"/>
+      <c r="C98" s="51"/>
       <c r="D98" s="29">
         <v>45</v>
       </c>
@@ -3079,13 +3085,13 @@
       <c r="F98" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G98" s="53"/>
+      <c r="G98" s="54"/>
       <c r="H98" s="22"/>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B99" s="4"/>
-      <c r="C99" s="50"/>
+      <c r="C99" s="51"/>
       <c r="D99" s="29">
         <v>90</v>
       </c>
@@ -3095,13 +3101,13 @@
       <c r="F99" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G99" s="53"/>
+      <c r="G99" s="54"/>
       <c r="H99" s="22"/>
       <c r="I99" s="5"/>
     </row>
     <row r="100" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B100" s="4"/>
-      <c r="C100" s="50"/>
+      <c r="C100" s="51"/>
       <c r="D100" s="29">
         <v>45</v>
       </c>
@@ -3111,13 +3117,13 @@
       <c r="F100" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="G100" s="53"/>
+      <c r="G100" s="54"/>
       <c r="H100" s="22"/>
       <c r="I100" s="5"/>
     </row>
     <row r="101" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="4"/>
-      <c r="C101" s="50"/>
+      <c r="C101" s="51"/>
       <c r="D101" s="29">
         <v>20</v>
       </c>
@@ -3127,13 +3133,13 @@
       <c r="F101" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G101" s="53"/>
+      <c r="G101" s="54"/>
       <c r="H101" s="22"/>
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B102" s="4"/>
-      <c r="C102" s="51"/>
+      <c r="C102" s="52"/>
       <c r="D102" s="29">
         <v>25</v>
       </c>
@@ -3143,7 +3149,7 @@
       <c r="F102" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G102" s="54"/>
+      <c r="G102" s="55"/>
       <c r="H102" s="22"/>
       <c r="I102" s="5"/>
     </row>
@@ -3164,7 +3170,7 @@
     </row>
     <row r="104" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B104" s="4"/>
-      <c r="C104" s="49">
+      <c r="C104" s="50">
         <v>43613</v>
       </c>
       <c r="D104" s="43">
@@ -3176,7 +3182,7 @@
       <c r="F104" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="G104" s="52" t="s">
+      <c r="G104" s="53" t="s">
         <v>164</v>
       </c>
       <c r="H104" s="47"/>
@@ -3184,7 +3190,7 @@
     </row>
     <row r="105" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B105" s="4"/>
-      <c r="C105" s="50"/>
+      <c r="C105" s="51"/>
       <c r="D105" s="43">
         <v>90</v>
       </c>
@@ -3194,13 +3200,13 @@
       <c r="F105" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="G105" s="53"/>
+      <c r="G105" s="54"/>
       <c r="H105" s="47"/>
       <c r="I105" s="5"/>
     </row>
     <row r="106" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B106" s="4"/>
-      <c r="C106" s="50"/>
+      <c r="C106" s="51"/>
       <c r="D106" s="43">
         <v>45</v>
       </c>
@@ -3210,13 +3216,13 @@
       <c r="F106" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="G106" s="53"/>
+      <c r="G106" s="54"/>
       <c r="H106" s="47"/>
       <c r="I106" s="5"/>
     </row>
     <row r="107" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B107" s="4"/>
-      <c r="C107" s="50"/>
+      <c r="C107" s="51"/>
       <c r="D107" s="43">
         <v>90</v>
       </c>
@@ -3226,13 +3232,13 @@
       <c r="F107" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="G107" s="53"/>
+      <c r="G107" s="54"/>
       <c r="H107" s="47"/>
       <c r="I107" s="5"/>
     </row>
     <row r="108" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B108" s="4"/>
-      <c r="C108" s="51"/>
+      <c r="C108" s="52"/>
       <c r="D108" s="43">
         <v>90</v>
       </c>
@@ -3242,7 +3248,7 @@
       <c r="F108" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="G108" s="54"/>
+      <c r="G108" s="55"/>
       <c r="H108" s="47"/>
       <c r="I108" s="5"/>
     </row>
@@ -3263,7 +3269,7 @@
     </row>
     <row r="110" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B110" s="4"/>
-      <c r="C110" s="49">
+      <c r="C110" s="50">
         <v>43614</v>
       </c>
       <c r="D110" s="43">
@@ -3283,12 +3289,12 @@
     </row>
     <row r="111" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B111" s="4"/>
-      <c r="C111" s="50"/>
+      <c r="C111" s="51"/>
       <c r="D111" s="43">
         <v>90</v>
       </c>
       <c r="E111" s="24" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="F111" s="45" t="s">
         <v>165</v>
@@ -3299,7 +3305,7 @@
     </row>
     <row r="112" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B112" s="4"/>
-      <c r="C112" s="51"/>
+      <c r="C112" s="52"/>
       <c r="D112" s="43">
         <v>45</v>
       </c>
@@ -3330,7 +3336,9 @@
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="4"/>
-      <c r="C114" s="48"/>
+      <c r="C114" s="48">
+        <v>43620</v>
+      </c>
       <c r="D114" s="43"/>
       <c r="E114" s="44"/>
       <c r="F114" s="45"/>
@@ -3339,25 +3347,175 @@
       <c r="I114" s="5"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B115" s="8"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="35"/>
-      <c r="E115" s="28"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="35"/>
-      <c r="H115" s="19"/>
-      <c r="I115" s="9"/>
-    </row>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="49"/>
+      <c r="D115" s="43"/>
+      <c r="E115" s="44"/>
+      <c r="F115" s="45"/>
+      <c r="G115" s="43"/>
+      <c r="H115" s="46"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B116" s="4"/>
+      <c r="C116" s="49"/>
+      <c r="D116" s="43"/>
+      <c r="E116" s="44"/>
+      <c r="F116" s="45"/>
+      <c r="G116" s="43"/>
+      <c r="H116" s="46"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B117" s="4"/>
+      <c r="C117" s="49"/>
+      <c r="D117" s="43"/>
+      <c r="E117" s="44"/>
+      <c r="F117" s="45"/>
+      <c r="G117" s="43"/>
+      <c r="H117" s="46"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B118" s="4"/>
+      <c r="C118" s="49"/>
+      <c r="D118" s="43"/>
+      <c r="E118" s="44"/>
+      <c r="F118" s="45"/>
+      <c r="G118" s="43"/>
+      <c r="H118" s="46"/>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B119" s="4"/>
+      <c r="C119" s="49"/>
+      <c r="D119" s="43"/>
+      <c r="E119" s="44"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="43"/>
+      <c r="H119" s="46"/>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B120" s="4"/>
+      <c r="C120" s="49"/>
+      <c r="D120" s="43"/>
+      <c r="E120" s="44"/>
+      <c r="F120" s="45"/>
+      <c r="G120" s="43"/>
+      <c r="H120" s="46"/>
+      <c r="I120" s="5"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B121" s="4"/>
+      <c r="C121" s="49"/>
+      <c r="D121" s="43"/>
+      <c r="E121" s="44"/>
+      <c r="F121" s="45"/>
+      <c r="G121" s="43"/>
+      <c r="H121" s="46"/>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B122" s="4"/>
+      <c r="C122" s="49"/>
+      <c r="D122" s="43"/>
+      <c r="E122" s="44"/>
+      <c r="F122" s="45"/>
+      <c r="G122" s="43"/>
+      <c r="H122" s="46"/>
+      <c r="I122" s="5"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B123" s="4"/>
+      <c r="C123" s="49"/>
+      <c r="D123" s="43"/>
+      <c r="E123" s="44"/>
+      <c r="F123" s="45"/>
+      <c r="G123" s="43"/>
+      <c r="H123" s="46"/>
+      <c r="I123" s="5"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="4"/>
+      <c r="C124" s="49"/>
+      <c r="D124" s="43"/>
+      <c r="E124" s="44"/>
+      <c r="F124" s="45"/>
+      <c r="G124" s="43"/>
+      <c r="H124" s="46"/>
+      <c r="I124" s="5"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B125" s="4"/>
+      <c r="C125" s="49"/>
+      <c r="D125" s="43"/>
+      <c r="E125" s="44"/>
+      <c r="F125" s="45"/>
+      <c r="G125" s="43"/>
+      <c r="H125" s="46"/>
+      <c r="I125" s="5"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B126" s="4"/>
+      <c r="C126" s="49"/>
+      <c r="D126" s="43"/>
+      <c r="E126" s="44"/>
+      <c r="F126" s="45"/>
+      <c r="G126" s="43"/>
+      <c r="H126" s="46"/>
+      <c r="I126" s="5"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B127" s="4"/>
+      <c r="C127" s="49"/>
+      <c r="D127" s="43"/>
+      <c r="E127" s="44"/>
+      <c r="F127" s="45"/>
+      <c r="G127" s="43"/>
+      <c r="H127" s="46"/>
+      <c r="I127" s="5"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="4"/>
+      <c r="C128" s="49"/>
+      <c r="D128" s="43"/>
+      <c r="E128" s="44"/>
+      <c r="F128" s="45"/>
+      <c r="G128" s="43"/>
+      <c r="H128" s="46"/>
+      <c r="I128" s="5"/>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B129" s="4"/>
+      <c r="C129" s="49"/>
+      <c r="D129" s="43"/>
+      <c r="E129" s="44"/>
+      <c r="F129" s="45"/>
+      <c r="G129" s="43"/>
+      <c r="H129" s="46"/>
+      <c r="I129" s="5"/>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B130" s="8"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="35"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="35"/>
+      <c r="H130" s="19"/>
+      <c r="I130" s="9"/>
+    </row>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="C104:C108"/>
-    <mergeCell ref="G104:G108"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="C52:C56"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G9:G16"/>
     <mergeCell ref="G18:G20"/>
@@ -3367,14 +3525,14 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="C104:C108"/>
+    <mergeCell ref="G104:G108"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="G110:G112"/>
     <mergeCell ref="C95:C102"/>
     <mergeCell ref="G95:G102"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="C52:C56"/>
     <mergeCell ref="C82:C85"/>
     <mergeCell ref="G75:G80"/>
     <mergeCell ref="G82:G85"/>

</xml_diff>

<commit_message>
Version finale de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="187">
   <si>
     <t>Activités</t>
   </si>
@@ -537,6 +537,54 @@
   </si>
   <si>
     <t>Diego Sanchez et Frédérique Andolfatto, Code</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Manuel d'installation</t>
+  </si>
+  <si>
+    <t>Création de mon manuel d'installation, en reprenant les points principale de mon projet</t>
+  </si>
+  <si>
+    <t>Création de mon manuel d'utilisation grâce à mon site en ligne</t>
+  </si>
+  <si>
+    <t>Fin du point de la conception et début de la réalisation dans mon rapport de projet</t>
+  </si>
+  <si>
+    <t>Suite et fin de ma documentation</t>
+  </si>
+  <si>
+    <t>Création et finalisation de mon script php pour le mail de rappel</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Glossaire</t>
+  </si>
+  <si>
+    <t>Création de mon glossaire qui sera en annexe de mon projet</t>
+  </si>
+  <si>
+    <t>quelques réglage graphique de mon site, qui affichait des tâches d'autres utilisateurs</t>
+  </si>
+  <si>
+    <t>Relecture de mon rapport de projet</t>
+  </si>
+  <si>
+    <t>04.06.2019, total durée</t>
+  </si>
+  <si>
+    <t>Grosse avancée de ma documentaion et de mes documents externes afin de finaliser mon projet</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Code et documentation</t>
+  </si>
+  <si>
+    <t>Finalisation du script pour le mail de rappel ainsi que création de la mise en installation du script dans le manuel d'installation</t>
+  </si>
+  <si>
+    <t>Documentation de mon code de projet</t>
   </si>
 </sst>
 </file>
@@ -1035,6 +1083,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1052,9 +1103,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1507,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M173"/>
+  <dimension ref="A1:M190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1528,31 +1576,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1614,7 +1662,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="61">
+      <c r="C9" s="62">
         <v>43592</v>
       </c>
       <c r="D9" s="39">
@@ -1626,7 +1674,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="61" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -2329,7 +2377,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="56" t="s">
+      <c r="G52" s="57" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="22"/>
@@ -2347,7 +2395,7 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="57"/>
+      <c r="G53" s="58"/>
       <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
@@ -2363,7 +2411,7 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="57"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
@@ -2379,7 +2427,7 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="57"/>
+      <c r="G55" s="58"/>
       <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
@@ -2395,7 +2443,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="58"/>
+      <c r="G56" s="59"/>
       <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
@@ -2821,7 +2869,7 @@
       <c r="F82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G82" s="56" t="s">
+      <c r="G82" s="57" t="s">
         <v>137</v>
       </c>
       <c r="H82" s="22"/>
@@ -2839,7 +2887,7 @@
       <c r="F83" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G83" s="57"/>
+      <c r="G83" s="58"/>
       <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
@@ -2855,7 +2903,7 @@
       <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="57"/>
+      <c r="G84" s="58"/>
       <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
@@ -2871,7 +2919,7 @@
       <c r="F85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G85" s="58"/>
+      <c r="G85" s="59"/>
       <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
@@ -3281,7 +3329,7 @@
       <c r="F110" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="G110" s="56" t="s">
+      <c r="G110" s="57" t="s">
         <v>169</v>
       </c>
       <c r="H110" s="47"/>
@@ -3299,7 +3347,7 @@
       <c r="F111" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="G111" s="57"/>
+      <c r="G111" s="58"/>
       <c r="H111" s="47"/>
       <c r="I111" s="5"/>
     </row>
@@ -3315,7 +3363,7 @@
       <c r="F112" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="G112" s="58"/>
+      <c r="G112" s="59"/>
       <c r="H112" s="47"/>
       <c r="I112" s="5"/>
     </row>
@@ -3334,121 +3382,190 @@
       <c r="H113" s="46"/>
       <c r="I113" s="5"/>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B114" s="4"/>
-      <c r="C114" s="48">
+      <c r="C114" s="50">
         <v>43620</v>
       </c>
-      <c r="D114" s="43"/>
-      <c r="E114" s="44"/>
-      <c r="F114" s="45"/>
-      <c r="G114" s="43"/>
-      <c r="H114" s="46"/>
+      <c r="D114" s="43">
+        <v>90</v>
+      </c>
+      <c r="E114" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F114" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="G114" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="H114" s="47"/>
       <c r="I114" s="5"/>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B115" s="4"/>
-      <c r="C115" s="49"/>
-      <c r="D115" s="43"/>
-      <c r="E115" s="44"/>
-      <c r="F115" s="45"/>
-      <c r="G115" s="43"/>
-      <c r="H115" s="46"/>
+      <c r="C115" s="51"/>
+      <c r="D115" s="43">
+        <v>90</v>
+      </c>
+      <c r="E115" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F115" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="G115" s="54"/>
+      <c r="H115" s="47"/>
       <c r="I115" s="5"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B116" s="4"/>
-      <c r="C116" s="49"/>
-      <c r="D116" s="43"/>
-      <c r="E116" s="44"/>
-      <c r="F116" s="45"/>
-      <c r="G116" s="43"/>
-      <c r="H116" s="46"/>
+      <c r="C116" s="51"/>
+      <c r="D116" s="43">
+        <v>45</v>
+      </c>
+      <c r="E116" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F116" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G116" s="54"/>
+      <c r="H116" s="47"/>
       <c r="I116" s="5"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="4"/>
-      <c r="C117" s="49"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="44"/>
-      <c r="F117" s="45"/>
-      <c r="G117" s="43"/>
-      <c r="H117" s="46"/>
+      <c r="C117" s="51"/>
+      <c r="D117" s="43">
+        <v>90</v>
+      </c>
+      <c r="E117" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F117" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="G117" s="54"/>
+      <c r="H117" s="47"/>
       <c r="I117" s="5"/>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B118" s="4"/>
-      <c r="C118" s="49"/>
-      <c r="D118" s="43"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="45"/>
-      <c r="G118" s="43"/>
-      <c r="H118" s="46"/>
+      <c r="C118" s="51"/>
+      <c r="D118" s="43">
+        <v>20</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F118" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="G118" s="54"/>
+      <c r="H118" s="47"/>
       <c r="I118" s="5"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B119" s="4"/>
-      <c r="C119" s="49"/>
-      <c r="D119" s="43"/>
-      <c r="E119" s="44"/>
-      <c r="F119" s="45"/>
-      <c r="G119" s="43"/>
-      <c r="H119" s="46"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="43">
+        <v>25</v>
+      </c>
+      <c r="E119" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F119" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="G119" s="54"/>
+      <c r="H119" s="47"/>
       <c r="I119" s="5"/>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B120" s="4"/>
-      <c r="C120" s="49"/>
-      <c r="D120" s="43"/>
-      <c r="E120" s="44"/>
-      <c r="F120" s="45"/>
-      <c r="G120" s="43"/>
-      <c r="H120" s="46"/>
+      <c r="C120" s="51"/>
+      <c r="D120" s="43">
+        <v>25</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F120" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="G120" s="54"/>
+      <c r="H120" s="47"/>
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="4"/>
-      <c r="C121" s="49"/>
-      <c r="D121" s="43"/>
-      <c r="E121" s="44"/>
-      <c r="F121" s="45"/>
-      <c r="G121" s="43"/>
-      <c r="H121" s="46"/>
+      <c r="C121" s="52"/>
+      <c r="D121" s="43">
+        <v>20</v>
+      </c>
+      <c r="E121" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F121" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G121" s="55"/>
+      <c r="H121" s="47"/>
       <c r="I121" s="5"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" s="4"/>
-      <c r="C122" s="49"/>
-      <c r="D122" s="43"/>
+      <c r="C122" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D122" s="43">
+        <f>SUM(D114:D121)</f>
+        <v>405</v>
+      </c>
       <c r="E122" s="44"/>
       <c r="F122" s="45"/>
       <c r="G122" s="43"/>
       <c r="H122" s="46"/>
       <c r="I122" s="5"/>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B123" s="4"/>
-      <c r="C123" s="49"/>
-      <c r="D123" s="43"/>
-      <c r="E123" s="44"/>
-      <c r="F123" s="45"/>
+      <c r="C123" s="48">
+        <v>43621</v>
+      </c>
+      <c r="D123" s="43">
+        <v>45</v>
+      </c>
+      <c r="E123" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F123" s="45" t="s">
+        <v>185</v>
+      </c>
       <c r="G123" s="43"/>
-      <c r="H123" s="46"/>
+      <c r="H123" s="47"/>
       <c r="I123" s="5"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="4"/>
-      <c r="C124" s="49"/>
-      <c r="D124" s="43"/>
-      <c r="E124" s="44"/>
-      <c r="F124" s="45"/>
+      <c r="C124" s="48"/>
+      <c r="D124" s="43">
+        <v>45</v>
+      </c>
+      <c r="E124" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F124" s="45" t="s">
+        <v>186</v>
+      </c>
       <c r="G124" s="43"/>
-      <c r="H124" s="46"/>
+      <c r="H124" s="47"/>
       <c r="I124" s="5"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="4"/>
-      <c r="C125" s="49"/>
+      <c r="C125" s="48"/>
       <c r="D125" s="43"/>
       <c r="E125" s="44"/>
       <c r="F125" s="45"/>
@@ -3458,7 +3575,7 @@
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="4"/>
-      <c r="C126" s="49"/>
+      <c r="C126" s="48"/>
       <c r="D126" s="43"/>
       <c r="E126" s="44"/>
       <c r="F126" s="45"/>
@@ -3468,7 +3585,7 @@
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="4"/>
-      <c r="C127" s="49"/>
+      <c r="C127" s="48"/>
       <c r="D127" s="43"/>
       <c r="E127" s="44"/>
       <c r="F127" s="45"/>
@@ -3478,7 +3595,7 @@
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="4"/>
-      <c r="C128" s="49"/>
+      <c r="C128" s="48"/>
       <c r="D128" s="43"/>
       <c r="E128" s="44"/>
       <c r="F128" s="45"/>
@@ -3488,7 +3605,7 @@
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="4"/>
-      <c r="C129" s="49"/>
+      <c r="C129" s="48"/>
       <c r="D129" s="43"/>
       <c r="E129" s="44"/>
       <c r="F129" s="45"/>
@@ -3497,34 +3614,191 @@
       <c r="I129" s="5"/>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B130" s="8"/>
-      <c r="C130" s="21"/>
-      <c r="D130" s="35"/>
-      <c r="E130" s="28"/>
-      <c r="F130" s="18"/>
-      <c r="G130" s="35"/>
-      <c r="H130" s="19"/>
-      <c r="I130" s="9"/>
-    </row>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="48"/>
+      <c r="D130" s="43"/>
+      <c r="E130" s="44"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="43"/>
+      <c r="H130" s="46"/>
+      <c r="I130" s="5"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B131" s="4"/>
+      <c r="C131" s="48"/>
+      <c r="D131" s="43"/>
+      <c r="E131" s="44"/>
+      <c r="F131" s="45"/>
+      <c r="G131" s="43"/>
+      <c r="H131" s="46"/>
+      <c r="I131" s="5"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B132" s="4"/>
+      <c r="C132" s="49"/>
+      <c r="D132" s="43"/>
+      <c r="E132" s="44"/>
+      <c r="F132" s="45"/>
+      <c r="G132" s="43"/>
+      <c r="H132" s="46"/>
+      <c r="I132" s="5"/>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B133" s="4"/>
+      <c r="C133" s="49"/>
+      <c r="D133" s="43"/>
+      <c r="E133" s="44"/>
+      <c r="F133" s="45"/>
+      <c r="G133" s="43"/>
+      <c r="H133" s="46"/>
+      <c r="I133" s="5"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B134" s="4"/>
+      <c r="C134" s="49"/>
+      <c r="D134" s="43"/>
+      <c r="E134" s="44"/>
+      <c r="F134" s="45"/>
+      <c r="G134" s="43"/>
+      <c r="H134" s="46"/>
+      <c r="I134" s="5"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B135" s="4"/>
+      <c r="C135" s="49"/>
+      <c r="D135" s="43"/>
+      <c r="E135" s="44"/>
+      <c r="F135" s="45"/>
+      <c r="G135" s="43"/>
+      <c r="H135" s="46"/>
+      <c r="I135" s="5"/>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B136" s="4"/>
+      <c r="C136" s="49"/>
+      <c r="D136" s="43"/>
+      <c r="E136" s="44"/>
+      <c r="F136" s="45"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="46"/>
+      <c r="I136" s="5"/>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B137" s="4"/>
+      <c r="C137" s="49"/>
+      <c r="D137" s="43"/>
+      <c r="E137" s="44"/>
+      <c r="F137" s="45"/>
+      <c r="G137" s="43"/>
+      <c r="H137" s="46"/>
+      <c r="I137" s="5"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B138" s="4"/>
+      <c r="C138" s="49"/>
+      <c r="D138" s="43"/>
+      <c r="E138" s="44"/>
+      <c r="F138" s="45"/>
+      <c r="G138" s="43"/>
+      <c r="H138" s="46"/>
+      <c r="I138" s="5"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B139" s="4"/>
+      <c r="C139" s="49"/>
+      <c r="D139" s="43"/>
+      <c r="E139" s="44"/>
+      <c r="F139" s="45"/>
+      <c r="G139" s="43"/>
+      <c r="H139" s="46"/>
+      <c r="I139" s="5"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B140" s="4"/>
+      <c r="C140" s="49"/>
+      <c r="D140" s="43"/>
+      <c r="E140" s="44"/>
+      <c r="F140" s="45"/>
+      <c r="G140" s="43"/>
+      <c r="H140" s="46"/>
+      <c r="I140" s="5"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B141" s="4"/>
+      <c r="C141" s="49"/>
+      <c r="D141" s="43"/>
+      <c r="E141" s="44"/>
+      <c r="F141" s="45"/>
+      <c r="G141" s="43"/>
+      <c r="H141" s="46"/>
+      <c r="I141" s="5"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B142" s="4"/>
+      <c r="C142" s="49"/>
+      <c r="D142" s="43"/>
+      <c r="E142" s="44"/>
+      <c r="F142" s="45"/>
+      <c r="G142" s="43"/>
+      <c r="H142" s="46"/>
+      <c r="I142" s="5"/>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B143" s="4"/>
+      <c r="C143" s="49"/>
+      <c r="D143" s="43"/>
+      <c r="E143" s="44"/>
+      <c r="F143" s="45"/>
+      <c r="G143" s="43"/>
+      <c r="H143" s="46"/>
+      <c r="I143" s="5"/>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B144" s="4"/>
+      <c r="C144" s="49"/>
+      <c r="D144" s="43"/>
+      <c r="E144" s="44"/>
+      <c r="F144" s="45"/>
+      <c r="G144" s="43"/>
+      <c r="H144" s="46"/>
+      <c r="I144" s="5"/>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B145" s="4"/>
+      <c r="C145" s="49"/>
+      <c r="D145" s="43"/>
+      <c r="E145" s="44"/>
+      <c r="F145" s="45"/>
+      <c r="G145" s="43"/>
+      <c r="H145" s="46"/>
+      <c r="I145" s="5"/>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B146" s="4"/>
+      <c r="C146" s="49"/>
+      <c r="D146" s="43"/>
+      <c r="E146" s="44"/>
+      <c r="F146" s="45"/>
+      <c r="G146" s="43"/>
+      <c r="H146" s="46"/>
+      <c r="I146" s="5"/>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B147" s="8"/>
+      <c r="C147" s="21"/>
+      <c r="D147" s="35"/>
+      <c r="E147" s="28"/>
+      <c r="F147" s="18"/>
+      <c r="G147" s="35"/>
+      <c r="H147" s="19"/>
+      <c r="I147" s="9"/>
+    </row>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="G9:G16"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="C9:C16"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="G22:G30"/>
+  <mergeCells count="33">
+    <mergeCell ref="C114:C121"/>
+    <mergeCell ref="G114:G121"/>
     <mergeCell ref="C58:C66"/>
     <mergeCell ref="G58:G66"/>
     <mergeCell ref="C104:C108"/>
@@ -3541,6 +3815,21 @@
     <mergeCell ref="C87:C93"/>
     <mergeCell ref="G87:G93"/>
     <mergeCell ref="G68:G73"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G9:G16"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="C9:C16"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="G22:G30"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="C52:C56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
version finale de la documentation et du code
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="195">
   <si>
     <t>Activités</t>
   </si>
@@ -585,6 +585,30 @@
   </si>
   <si>
     <t>Documentation de mon code de projet</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Résumé</t>
+  </si>
+  <si>
+    <t>Finalisation de mon résumé de fin de projet</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Relecture</t>
+  </si>
+  <si>
+    <t>Diego Sanchez, Impression</t>
+  </si>
+  <si>
+    <t>Relecture finale de mon projet et des divers documents annexes</t>
+  </si>
+  <si>
+    <t>Impression de mes documents</t>
+  </si>
+  <si>
+    <t>05.06.2019, total durée</t>
+  </si>
+  <si>
+    <t>Finalisation et impression de mon projet</t>
   </si>
 </sst>
 </file>
@@ -936,7 +960,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1062,12 +1086,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1083,6 +1101,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,15 +1120,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1555,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M190"/>
+  <dimension ref="A1:M172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1576,31 +1594,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="56"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1662,7 +1680,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="62">
+      <c r="C9" s="56">
         <v>43592</v>
       </c>
       <c r="D9" s="39">
@@ -1674,7 +1692,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="55" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -1682,7 +1700,7 @@
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="29">
         <v>75</v>
       </c>
@@ -1692,13 +1710,13 @@
       <c r="F10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="54"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="22"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="51"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="29">
         <v>45</v>
       </c>
@@ -1708,13 +1726,13 @@
       <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="54"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="22"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="29">
         <v>75</v>
       </c>
@@ -1724,13 +1742,13 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="54"/>
+      <c r="G12" s="52"/>
       <c r="H12" s="22"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="51"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="29">
         <v>15</v>
       </c>
@@ -1740,13 +1758,13 @@
       <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="54"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="22"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="29">
         <v>30</v>
       </c>
@@ -1756,13 +1774,13 @@
       <c r="F14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="52"/>
       <c r="H14" s="22"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="51"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="29">
         <v>75</v>
       </c>
@@ -1772,13 +1790,13 @@
       <c r="F15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54"/>
+      <c r="G15" s="52"/>
       <c r="H15" s="22"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="52"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="29">
         <v>30</v>
       </c>
@@ -1788,7 +1806,7 @@
       <c r="F16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="22"/>
       <c r="I16" s="5"/>
     </row>
@@ -1809,7 +1827,7 @@
     </row>
     <row r="18" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="50">
+      <c r="C18" s="48">
         <v>43593</v>
       </c>
       <c r="D18" s="29">
@@ -1821,7 +1839,7 @@
       <c r="F18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="51" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="22"/>
@@ -1829,7 +1847,7 @@
     </row>
     <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="29">
         <v>90</v>
       </c>
@@ -1839,13 +1857,13 @@
       <c r="F19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="54"/>
+      <c r="G19" s="52"/>
       <c r="H19" s="22"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
-      <c r="C20" s="52"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="29">
         <v>45</v>
       </c>
@@ -1855,7 +1873,7 @@
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="55"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="22"/>
       <c r="I20" s="5"/>
     </row>
@@ -1876,7 +1894,7 @@
     </row>
     <row r="22" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="C22" s="50">
+      <c r="C22" s="48">
         <v>43594</v>
       </c>
       <c r="D22" s="29">
@@ -1888,7 +1906,7 @@
       <c r="F22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="51" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="22"/>
@@ -1896,7 +1914,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="51"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="29">
         <v>30</v>
       </c>
@@ -1906,13 +1924,13 @@
       <c r="F23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="52"/>
       <c r="H23" s="22"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="C24" s="51"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="29">
         <v>70</v>
       </c>
@@ -1922,13 +1940,13 @@
       <c r="F24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="52"/>
       <c r="H24" s="22"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="51"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="29">
         <v>35</v>
       </c>
@@ -1938,13 +1956,13 @@
       <c r="F25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="54"/>
+      <c r="G25" s="52"/>
       <c r="H25" s="22"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
-      <c r="C26" s="51"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="29">
         <v>20</v>
       </c>
@@ -1954,13 +1972,13 @@
       <c r="F26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="54"/>
+      <c r="G26" s="52"/>
       <c r="H26" s="22"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="51"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="29">
         <v>45</v>
       </c>
@@ -1970,13 +1988,13 @@
       <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="52"/>
       <c r="H27" s="22"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="51"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="29">
         <v>55</v>
       </c>
@@ -1986,13 +2004,13 @@
       <c r="F28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="54"/>
+      <c r="G28" s="52"/>
       <c r="H28" s="22"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="51"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="29">
         <v>70</v>
       </c>
@@ -2002,13 +2020,13 @@
       <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="54"/>
+      <c r="G29" s="52"/>
       <c r="H29" s="22"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="52"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="29">
         <v>20</v>
       </c>
@@ -2018,7 +2036,7 @@
       <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="55"/>
+      <c r="G30" s="53"/>
       <c r="H30" s="22"/>
       <c r="I30" s="5"/>
     </row>
@@ -2039,7 +2057,7 @@
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="50">
+      <c r="C32" s="48">
         <v>43595</v>
       </c>
       <c r="D32" s="29">
@@ -2051,7 +2069,7 @@
       <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="51" t="s">
         <v>65</v>
       </c>
       <c r="H32" s="22"/>
@@ -2059,7 +2077,7 @@
     </row>
     <row r="33" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
-      <c r="C33" s="51"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="29">
         <v>45</v>
       </c>
@@ -2069,13 +2087,13 @@
       <c r="F33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="54"/>
+      <c r="G33" s="52"/>
       <c r="H33" s="22"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="51"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="29">
         <v>70</v>
       </c>
@@ -2085,13 +2103,13 @@
       <c r="F34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="54"/>
+      <c r="G34" s="52"/>
       <c r="H34" s="22"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
-      <c r="C35" s="51"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="29">
         <v>90</v>
       </c>
@@ -2101,13 +2119,13 @@
       <c r="F35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="52"/>
       <c r="H35" s="22"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="51"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="29">
         <v>45</v>
       </c>
@@ -2117,13 +2135,13 @@
       <c r="F36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="54"/>
+      <c r="G36" s="52"/>
       <c r="H36" s="22"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="51"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="29">
         <v>20</v>
       </c>
@@ -2133,13 +2151,13 @@
       <c r="F37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="54"/>
+      <c r="G37" s="52"/>
       <c r="H37" s="22"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="52"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="29">
         <v>25</v>
       </c>
@@ -2149,7 +2167,7 @@
       <c r="F38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="55"/>
+      <c r="G38" s="53"/>
       <c r="H38" s="22"/>
       <c r="I38" s="5"/>
     </row>
@@ -2170,7 +2188,7 @@
     </row>
     <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="50">
+      <c r="C40" s="48">
         <v>43599</v>
       </c>
       <c r="D40" s="29">
@@ -2182,7 +2200,7 @@
       <c r="F40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="51" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="22"/>
@@ -2190,7 +2208,7 @@
     </row>
     <row r="41" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="51"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="29">
         <v>15</v>
       </c>
@@ -2200,13 +2218,13 @@
       <c r="F41" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="54"/>
+      <c r="G41" s="52"/>
       <c r="H41" s="22"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="C42" s="51"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="29">
         <v>45</v>
       </c>
@@ -2216,13 +2234,13 @@
       <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="54"/>
+      <c r="G42" s="52"/>
       <c r="H42" s="22"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
-      <c r="C43" s="51"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="29">
         <v>45</v>
       </c>
@@ -2232,13 +2250,13 @@
       <c r="F43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="54"/>
+      <c r="G43" s="52"/>
       <c r="H43" s="22"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="51"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="29">
         <v>45</v>
       </c>
@@ -2248,13 +2266,13 @@
       <c r="F44" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="54"/>
+      <c r="G44" s="52"/>
       <c r="H44" s="22"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="C45" s="51"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="29">
         <v>45</v>
       </c>
@@ -2264,13 +2282,13 @@
       <c r="F45" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="54"/>
+      <c r="G45" s="52"/>
       <c r="H45" s="22"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="51"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="29">
         <v>45</v>
       </c>
@@ -2280,13 +2298,13 @@
       <c r="F46" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="54"/>
+      <c r="G46" s="52"/>
       <c r="H46" s="22"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="51"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="29">
         <v>45</v>
       </c>
@@ -2296,13 +2314,13 @@
       <c r="F47" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="54"/>
+      <c r="G47" s="52"/>
       <c r="H47" s="22"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="51"/>
+      <c r="C48" s="49"/>
       <c r="D48" s="29">
         <v>15</v>
       </c>
@@ -2312,13 +2330,13 @@
       <c r="F48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="54"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="22"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="51"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="29">
         <v>30</v>
       </c>
@@ -2328,13 +2346,13 @@
       <c r="F49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G49" s="54"/>
+      <c r="G49" s="52"/>
       <c r="H49" s="22"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="52"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="29">
         <v>45</v>
       </c>
@@ -2344,7 +2362,7 @@
       <c r="F50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="55"/>
+      <c r="G50" s="53"/>
       <c r="H50" s="22"/>
       <c r="I50" s="5"/>
     </row>
@@ -2365,7 +2383,7 @@
     </row>
     <row r="52" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
-      <c r="C52" s="50">
+      <c r="C52" s="48">
         <v>43600</v>
       </c>
       <c r="D52" s="29">
@@ -2377,7 +2395,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="57" t="s">
+      <c r="G52" s="58" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="22"/>
@@ -2385,7 +2403,7 @@
     </row>
     <row r="53" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
-      <c r="C53" s="51"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="29">
         <v>60</v>
       </c>
@@ -2395,13 +2413,13 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="58"/>
+      <c r="G53" s="59"/>
       <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
-      <c r="C54" s="51"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="29">
         <v>45</v>
       </c>
@@ -2411,13 +2429,13 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="58"/>
+      <c r="G54" s="59"/>
       <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
-      <c r="C55" s="51"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="29">
         <v>15</v>
       </c>
@@ -2427,13 +2445,13 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="58"/>
+      <c r="G55" s="59"/>
       <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
-      <c r="C56" s="52"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="29">
         <v>45</v>
       </c>
@@ -2443,7 +2461,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="59"/>
+      <c r="G56" s="60"/>
       <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
@@ -2464,7 +2482,7 @@
     </row>
     <row r="58" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
-      <c r="C58" s="50">
+      <c r="C58" s="48">
         <v>43601</v>
       </c>
       <c r="D58" s="29">
@@ -2476,7 +2494,7 @@
       <c r="F58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="53" t="s">
+      <c r="G58" s="51" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="22"/>
@@ -2484,7 +2502,7 @@
     </row>
     <row r="59" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="51"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="29">
         <v>15</v>
       </c>
@@ -2494,13 +2512,13 @@
       <c r="F59" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="54"/>
+      <c r="G59" s="52"/>
       <c r="H59" s="22"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
-      <c r="C60" s="51"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="29">
         <v>45</v>
       </c>
@@ -2510,13 +2528,13 @@
       <c r="F60" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="54"/>
+      <c r="G60" s="52"/>
       <c r="H60" s="22"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="51"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="29">
         <v>90</v>
       </c>
@@ -2526,13 +2544,13 @@
       <c r="F61" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="54"/>
+      <c r="G61" s="52"/>
       <c r="H61" s="22"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
-      <c r="C62" s="51"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="43">
         <v>30</v>
       </c>
@@ -2542,13 +2560,13 @@
       <c r="F62" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="54"/>
+      <c r="G62" s="52"/>
       <c r="H62" s="47"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
-      <c r="C63" s="51"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="29">
         <v>15</v>
       </c>
@@ -2558,13 +2576,13 @@
       <c r="F63" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G63" s="54"/>
+      <c r="G63" s="52"/>
       <c r="H63" s="22"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
-      <c r="C64" s="51"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="29">
         <v>45</v>
       </c>
@@ -2574,13 +2592,13 @@
       <c r="F64" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="54"/>
+      <c r="G64" s="52"/>
       <c r="H64" s="22"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
-      <c r="C65" s="51"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="29">
         <v>45</v>
       </c>
@@ -2590,13 +2608,13 @@
       <c r="F65" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="54"/>
+      <c r="G65" s="52"/>
       <c r="H65" s="22"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="52"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="29">
         <v>90</v>
       </c>
@@ -2606,7 +2624,7 @@
       <c r="F66" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="55"/>
+      <c r="G66" s="53"/>
       <c r="H66" s="22"/>
       <c r="I66" s="5"/>
     </row>
@@ -2627,7 +2645,7 @@
     </row>
     <row r="68" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="50">
+      <c r="C68" s="48">
         <v>43602</v>
       </c>
       <c r="D68" s="29">
@@ -2639,7 +2657,7 @@
       <c r="F68" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="53" t="s">
+      <c r="G68" s="51" t="s">
         <v>120</v>
       </c>
       <c r="H68" s="22"/>
@@ -2647,7 +2665,7 @@
     </row>
     <row r="69" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="51"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="29">
         <v>45</v>
       </c>
@@ -2657,13 +2675,13 @@
       <c r="F69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="54"/>
+      <c r="G69" s="52"/>
       <c r="H69" s="22"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="51"/>
+      <c r="C70" s="49"/>
       <c r="D70" s="29">
         <v>45</v>
       </c>
@@ -2673,13 +2691,13 @@
       <c r="F70" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="54"/>
+      <c r="G70" s="52"/>
       <c r="H70" s="22"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="51"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="29">
         <v>45</v>
       </c>
@@ -2689,13 +2707,13 @@
       <c r="F71" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G71" s="54"/>
+      <c r="G71" s="52"/>
       <c r="H71" s="22"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="51"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="43">
         <v>45</v>
       </c>
@@ -2705,13 +2723,13 @@
       <c r="F72" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="54"/>
+      <c r="G72" s="52"/>
       <c r="H72" s="47"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="52"/>
+      <c r="C73" s="50"/>
       <c r="D73" s="29">
         <v>90</v>
       </c>
@@ -2721,7 +2739,7 @@
       <c r="F73" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="55"/>
+      <c r="G73" s="53"/>
       <c r="H73" s="22"/>
       <c r="I73" s="5"/>
     </row>
@@ -2742,7 +2760,7 @@
     </row>
     <row r="75" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="50">
+      <c r="C75" s="48">
         <v>43606</v>
       </c>
       <c r="D75" s="29">
@@ -2754,7 +2772,7 @@
       <c r="F75" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G75" s="53" t="s">
+      <c r="G75" s="51" t="s">
         <v>136</v>
       </c>
       <c r="H75" s="22"/>
@@ -2762,7 +2780,7 @@
     </row>
     <row r="76" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="51"/>
+      <c r="C76" s="49"/>
       <c r="D76" s="43">
         <v>90</v>
       </c>
@@ -2772,13 +2790,13 @@
       <c r="F76" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="54"/>
+      <c r="G76" s="52"/>
       <c r="H76" s="47"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="51"/>
+      <c r="C77" s="49"/>
       <c r="D77" s="29">
         <v>45</v>
       </c>
@@ -2788,13 +2806,13 @@
       <c r="F77" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="54"/>
+      <c r="G77" s="52"/>
       <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="51"/>
+      <c r="C78" s="49"/>
       <c r="D78" s="43">
         <v>90</v>
       </c>
@@ -2804,13 +2822,13 @@
       <c r="F78" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G78" s="54"/>
+      <c r="G78" s="52"/>
       <c r="H78" s="47"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="51"/>
+      <c r="C79" s="49"/>
       <c r="D79" s="29">
         <v>90</v>
       </c>
@@ -2820,13 +2838,13 @@
       <c r="F79" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="54"/>
+      <c r="G79" s="52"/>
       <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="52"/>
+      <c r="C80" s="50"/>
       <c r="D80" s="29">
         <v>45</v>
       </c>
@@ -2836,7 +2854,7 @@
       <c r="F80" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G80" s="55"/>
+      <c r="G80" s="53"/>
       <c r="H80" s="22"/>
       <c r="I80" s="5"/>
     </row>
@@ -2857,7 +2875,7 @@
     </row>
     <row r="82" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="50">
+      <c r="C82" s="48">
         <v>43607</v>
       </c>
       <c r="D82" s="29">
@@ -2869,7 +2887,7 @@
       <c r="F82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G82" s="57" t="s">
+      <c r="G82" s="58" t="s">
         <v>137</v>
       </c>
       <c r="H82" s="22"/>
@@ -2877,7 +2895,7 @@
     </row>
     <row r="83" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="51"/>
+      <c r="C83" s="49"/>
       <c r="D83" s="29">
         <v>45</v>
       </c>
@@ -2887,13 +2905,13 @@
       <c r="F83" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G83" s="58"/>
+      <c r="G83" s="59"/>
       <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
-      <c r="C84" s="51"/>
+      <c r="C84" s="49"/>
       <c r="D84" s="29">
         <v>90</v>
       </c>
@@ -2903,13 +2921,13 @@
       <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="58"/>
+      <c r="G84" s="59"/>
       <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
-      <c r="C85" s="51"/>
+      <c r="C85" s="49"/>
       <c r="D85" s="29">
         <v>45</v>
       </c>
@@ -2919,7 +2937,7 @@
       <c r="F85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G85" s="59"/>
+      <c r="G85" s="60"/>
       <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
@@ -2940,7 +2958,7 @@
     </row>
     <row r="87" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B87" s="4"/>
-      <c r="C87" s="50">
+      <c r="C87" s="48">
         <v>43608</v>
       </c>
       <c r="D87" s="29">
@@ -2952,7 +2970,7 @@
       <c r="F87" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G87" s="53" t="s">
+      <c r="G87" s="51" t="s">
         <v>146</v>
       </c>
       <c r="H87" s="22"/>
@@ -2960,7 +2978,7 @@
     </row>
     <row r="88" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B88" s="4"/>
-      <c r="C88" s="51"/>
+      <c r="C88" s="49"/>
       <c r="D88" s="29">
         <v>70</v>
       </c>
@@ -2970,13 +2988,13 @@
       <c r="F88" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G88" s="54"/>
+      <c r="G88" s="52"/>
       <c r="H88" s="22"/>
       <c r="I88" s="5"/>
     </row>
     <row r="89" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B89" s="4"/>
-      <c r="C89" s="51"/>
+      <c r="C89" s="49"/>
       <c r="D89" s="29">
         <v>55</v>
       </c>
@@ -2986,13 +3004,13 @@
       <c r="F89" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="G89" s="54"/>
+      <c r="G89" s="52"/>
       <c r="H89" s="22"/>
       <c r="I89" s="5"/>
     </row>
     <row r="90" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B90" s="4"/>
-      <c r="C90" s="51"/>
+      <c r="C90" s="49"/>
       <c r="D90" s="29">
         <v>55</v>
       </c>
@@ -3002,13 +3020,13 @@
       <c r="F90" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="54"/>
+      <c r="G90" s="52"/>
       <c r="H90" s="22"/>
       <c r="I90" s="5"/>
     </row>
     <row r="91" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B91" s="4"/>
-      <c r="C91" s="51"/>
+      <c r="C91" s="49"/>
       <c r="D91" s="29">
         <v>90</v>
       </c>
@@ -3018,13 +3036,13 @@
       <c r="F91" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G91" s="54"/>
+      <c r="G91" s="52"/>
       <c r="H91" s="22"/>
       <c r="I91" s="5"/>
     </row>
     <row r="92" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
-      <c r="C92" s="51"/>
+      <c r="C92" s="49"/>
       <c r="D92" s="29">
         <v>45</v>
       </c>
@@ -3034,13 +3052,13 @@
       <c r="F92" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G92" s="54"/>
+      <c r="G92" s="52"/>
       <c r="H92" s="22"/>
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B93" s="4"/>
-      <c r="C93" s="52"/>
+      <c r="C93" s="50"/>
       <c r="D93" s="29">
         <v>45</v>
       </c>
@@ -3050,7 +3068,7 @@
       <c r="F93" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="G93" s="55"/>
+      <c r="G93" s="53"/>
       <c r="H93" s="22"/>
       <c r="I93" s="5"/>
     </row>
@@ -3071,7 +3089,7 @@
     </row>
     <row r="95" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B95" s="4"/>
-      <c r="C95" s="50">
+      <c r="C95" s="48">
         <v>43609</v>
       </c>
       <c r="D95" s="29">
@@ -3083,7 +3101,7 @@
       <c r="F95" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="G95" s="53" t="s">
+      <c r="G95" s="51" t="s">
         <v>157</v>
       </c>
       <c r="H95" s="22"/>
@@ -3091,7 +3109,7 @@
     </row>
     <row r="96" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B96" s="4"/>
-      <c r="C96" s="51"/>
+      <c r="C96" s="49"/>
       <c r="D96" s="29">
         <v>15</v>
       </c>
@@ -3101,13 +3119,13 @@
       <c r="F96" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G96" s="54"/>
+      <c r="G96" s="52"/>
       <c r="H96" s="22"/>
       <c r="I96" s="5"/>
     </row>
     <row r="97" spans="2:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B97" s="4"/>
-      <c r="C97" s="51"/>
+      <c r="C97" s="49"/>
       <c r="D97" s="29">
         <v>45</v>
       </c>
@@ -3117,13 +3135,13 @@
       <c r="F97" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G97" s="54"/>
+      <c r="G97" s="52"/>
       <c r="H97" s="22"/>
       <c r="I97" s="5"/>
     </row>
     <row r="98" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B98" s="4"/>
-      <c r="C98" s="51"/>
+      <c r="C98" s="49"/>
       <c r="D98" s="29">
         <v>45</v>
       </c>
@@ -3133,13 +3151,13 @@
       <c r="F98" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G98" s="54"/>
+      <c r="G98" s="52"/>
       <c r="H98" s="22"/>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B99" s="4"/>
-      <c r="C99" s="51"/>
+      <c r="C99" s="49"/>
       <c r="D99" s="29">
         <v>90</v>
       </c>
@@ -3149,13 +3167,13 @@
       <c r="F99" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G99" s="54"/>
+      <c r="G99" s="52"/>
       <c r="H99" s="22"/>
       <c r="I99" s="5"/>
     </row>
     <row r="100" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B100" s="4"/>
-      <c r="C100" s="51"/>
+      <c r="C100" s="49"/>
       <c r="D100" s="29">
         <v>45</v>
       </c>
@@ -3165,13 +3183,13 @@
       <c r="F100" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="G100" s="54"/>
+      <c r="G100" s="52"/>
       <c r="H100" s="22"/>
       <c r="I100" s="5"/>
     </row>
     <row r="101" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="4"/>
-      <c r="C101" s="51"/>
+      <c r="C101" s="49"/>
       <c r="D101" s="29">
         <v>20</v>
       </c>
@@ -3181,13 +3199,13 @@
       <c r="F101" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G101" s="54"/>
+      <c r="G101" s="52"/>
       <c r="H101" s="22"/>
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B102" s="4"/>
-      <c r="C102" s="52"/>
+      <c r="C102" s="50"/>
       <c r="D102" s="29">
         <v>25</v>
       </c>
@@ -3197,7 +3215,7 @@
       <c r="F102" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G102" s="55"/>
+      <c r="G102" s="53"/>
       <c r="H102" s="22"/>
       <c r="I102" s="5"/>
     </row>
@@ -3218,7 +3236,7 @@
     </row>
     <row r="104" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B104" s="4"/>
-      <c r="C104" s="50">
+      <c r="C104" s="48">
         <v>43613</v>
       </c>
       <c r="D104" s="43">
@@ -3230,7 +3248,7 @@
       <c r="F104" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="G104" s="53" t="s">
+      <c r="G104" s="51" t="s">
         <v>164</v>
       </c>
       <c r="H104" s="47"/>
@@ -3238,7 +3256,7 @@
     </row>
     <row r="105" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B105" s="4"/>
-      <c r="C105" s="51"/>
+      <c r="C105" s="49"/>
       <c r="D105" s="43">
         <v>90</v>
       </c>
@@ -3248,13 +3266,13 @@
       <c r="F105" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="G105" s="54"/>
+      <c r="G105" s="52"/>
       <c r="H105" s="47"/>
       <c r="I105" s="5"/>
     </row>
     <row r="106" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B106" s="4"/>
-      <c r="C106" s="51"/>
+      <c r="C106" s="49"/>
       <c r="D106" s="43">
         <v>45</v>
       </c>
@@ -3264,13 +3282,13 @@
       <c r="F106" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="G106" s="54"/>
+      <c r="G106" s="52"/>
       <c r="H106" s="47"/>
       <c r="I106" s="5"/>
     </row>
     <row r="107" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B107" s="4"/>
-      <c r="C107" s="51"/>
+      <c r="C107" s="49"/>
       <c r="D107" s="43">
         <v>90</v>
       </c>
@@ -3280,13 +3298,13 @@
       <c r="F107" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="G107" s="54"/>
+      <c r="G107" s="52"/>
       <c r="H107" s="47"/>
       <c r="I107" s="5"/>
     </row>
     <row r="108" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B108" s="4"/>
-      <c r="C108" s="52"/>
+      <c r="C108" s="50"/>
       <c r="D108" s="43">
         <v>90</v>
       </c>
@@ -3296,7 +3314,7 @@
       <c r="F108" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="G108" s="55"/>
+      <c r="G108" s="53"/>
       <c r="H108" s="47"/>
       <c r="I108" s="5"/>
     </row>
@@ -3317,7 +3335,7 @@
     </row>
     <row r="110" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B110" s="4"/>
-      <c r="C110" s="50">
+      <c r="C110" s="48">
         <v>43614</v>
       </c>
       <c r="D110" s="43">
@@ -3329,7 +3347,7 @@
       <c r="F110" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="G110" s="57" t="s">
+      <c r="G110" s="58" t="s">
         <v>169</v>
       </c>
       <c r="H110" s="47"/>
@@ -3337,7 +3355,7 @@
     </row>
     <row r="111" spans="2:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B111" s="4"/>
-      <c r="C111" s="51"/>
+      <c r="C111" s="49"/>
       <c r="D111" s="43">
         <v>90</v>
       </c>
@@ -3347,13 +3365,13 @@
       <c r="F111" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="G111" s="58"/>
+      <c r="G111" s="59"/>
       <c r="H111" s="47"/>
       <c r="I111" s="5"/>
     </row>
     <row r="112" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B112" s="4"/>
-      <c r="C112" s="52"/>
+      <c r="C112" s="50"/>
       <c r="D112" s="43">
         <v>45</v>
       </c>
@@ -3363,7 +3381,7 @@
       <c r="F112" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="G112" s="59"/>
+      <c r="G112" s="60"/>
       <c r="H112" s="47"/>
       <c r="I112" s="5"/>
     </row>
@@ -3384,7 +3402,7 @@
     </row>
     <row r="114" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B114" s="4"/>
-      <c r="C114" s="50">
+      <c r="C114" s="48">
         <v>43620</v>
       </c>
       <c r="D114" s="43">
@@ -3396,7 +3414,7 @@
       <c r="F114" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="G114" s="53" t="s">
+      <c r="G114" s="51" t="s">
         <v>183</v>
       </c>
       <c r="H114" s="47"/>
@@ -3404,7 +3422,7 @@
     </row>
     <row r="115" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B115" s="4"/>
-      <c r="C115" s="51"/>
+      <c r="C115" s="49"/>
       <c r="D115" s="43">
         <v>90</v>
       </c>
@@ -3414,13 +3432,13 @@
       <c r="F115" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="G115" s="54"/>
+      <c r="G115" s="52"/>
       <c r="H115" s="47"/>
       <c r="I115" s="5"/>
     </row>
     <row r="116" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B116" s="4"/>
-      <c r="C116" s="51"/>
+      <c r="C116" s="49"/>
       <c r="D116" s="43">
         <v>45</v>
       </c>
@@ -3430,13 +3448,13 @@
       <c r="F116" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="G116" s="54"/>
+      <c r="G116" s="52"/>
       <c r="H116" s="47"/>
       <c r="I116" s="5"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="4"/>
-      <c r="C117" s="51"/>
+      <c r="C117" s="49"/>
       <c r="D117" s="43">
         <v>90</v>
       </c>
@@ -3446,13 +3464,13 @@
       <c r="F117" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="G117" s="54"/>
+      <c r="G117" s="52"/>
       <c r="H117" s="47"/>
       <c r="I117" s="5"/>
     </row>
     <row r="118" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B118" s="4"/>
-      <c r="C118" s="51"/>
+      <c r="C118" s="49"/>
       <c r="D118" s="43">
         <v>20</v>
       </c>
@@ -3462,13 +3480,13 @@
       <c r="F118" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="G118" s="54"/>
+      <c r="G118" s="52"/>
       <c r="H118" s="47"/>
       <c r="I118" s="5"/>
     </row>
     <row r="119" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B119" s="4"/>
-      <c r="C119" s="51"/>
+      <c r="C119" s="49"/>
       <c r="D119" s="43">
         <v>25</v>
       </c>
@@ -3478,13 +3496,13 @@
       <c r="F119" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="G119" s="54"/>
+      <c r="G119" s="52"/>
       <c r="H119" s="47"/>
       <c r="I119" s="5"/>
     </row>
     <row r="120" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B120" s="4"/>
-      <c r="C120" s="51"/>
+      <c r="C120" s="49"/>
       <c r="D120" s="43">
         <v>25</v>
       </c>
@@ -3494,13 +3512,13 @@
       <c r="F120" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="G120" s="54"/>
+      <c r="G120" s="52"/>
       <c r="H120" s="47"/>
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="4"/>
-      <c r="C121" s="52"/>
+      <c r="C121" s="50"/>
       <c r="D121" s="43">
         <v>20</v>
       </c>
@@ -3510,7 +3528,7 @@
       <c r="F121" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="G121" s="55"/>
+      <c r="G121" s="53"/>
       <c r="H121" s="47"/>
       <c r="I121" s="5"/>
     </row>
@@ -3543,13 +3561,15 @@
       <c r="F123" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="G123" s="43"/>
+      <c r="G123" s="51" t="s">
+        <v>194</v>
+      </c>
       <c r="H123" s="47"/>
       <c r="I123" s="5"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="4"/>
-      <c r="C124" s="48"/>
+      <c r="C124" s="49"/>
       <c r="D124" s="43">
         <v>45</v>
       </c>
@@ -3559,44 +3579,67 @@
       <c r="F124" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="G124" s="43"/>
+      <c r="G124" s="52"/>
       <c r="H124" s="47"/>
       <c r="I124" s="5"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="4"/>
-      <c r="C125" s="48"/>
-      <c r="D125" s="43"/>
-      <c r="E125" s="44"/>
-      <c r="F125" s="45"/>
-      <c r="G125" s="43"/>
-      <c r="H125" s="46"/>
+      <c r="C125" s="49"/>
+      <c r="D125" s="43">
+        <v>45</v>
+      </c>
+      <c r="E125" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F125" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="G125" s="52"/>
+      <c r="H125" s="47"/>
       <c r="I125" s="5"/>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B126" s="4"/>
-      <c r="C126" s="48"/>
-      <c r="D126" s="43"/>
-      <c r="E126" s="44"/>
-      <c r="F126" s="45"/>
-      <c r="G126" s="43"/>
-      <c r="H126" s="46"/>
+      <c r="C126" s="49"/>
+      <c r="D126" s="43">
+        <v>45</v>
+      </c>
+      <c r="E126" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="F126" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G126" s="52"/>
+      <c r="H126" s="47"/>
       <c r="I126" s="5"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="4"/>
-      <c r="C127" s="48"/>
-      <c r="D127" s="43"/>
-      <c r="E127" s="44"/>
-      <c r="F127" s="45"/>
-      <c r="G127" s="43"/>
-      <c r="H127" s="46"/>
+      <c r="C127" s="50"/>
+      <c r="D127" s="43">
+        <v>45</v>
+      </c>
+      <c r="E127" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="F127" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="G127" s="53"/>
+      <c r="H127" s="47"/>
       <c r="I127" s="5"/>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="4"/>
-      <c r="C128" s="48"/>
-      <c r="D128" s="43"/>
+      <c r="C128" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D128" s="43">
+        <f>SUM(D123:D127)</f>
+        <v>225</v>
+      </c>
       <c r="E128" s="44"/>
       <c r="F128" s="45"/>
       <c r="G128" s="43"/>
@@ -3604,199 +3647,24 @@
       <c r="I128" s="5"/>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B129" s="4"/>
-      <c r="C129" s="48"/>
-      <c r="D129" s="43"/>
-      <c r="E129" s="44"/>
-      <c r="F129" s="45"/>
-      <c r="G129" s="43"/>
-      <c r="H129" s="46"/>
-      <c r="I129" s="5"/>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B130" s="4"/>
-      <c r="C130" s="48"/>
-      <c r="D130" s="43"/>
-      <c r="E130" s="44"/>
-      <c r="F130" s="45"/>
-      <c r="G130" s="43"/>
-      <c r="H130" s="46"/>
-      <c r="I130" s="5"/>
-    </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B131" s="4"/>
-      <c r="C131" s="48"/>
-      <c r="D131" s="43"/>
-      <c r="E131" s="44"/>
-      <c r="F131" s="45"/>
-      <c r="G131" s="43"/>
-      <c r="H131" s="46"/>
-      <c r="I131" s="5"/>
-    </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B132" s="4"/>
-      <c r="C132" s="49"/>
-      <c r="D132" s="43"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="45"/>
-      <c r="G132" s="43"/>
-      <c r="H132" s="46"/>
-      <c r="I132" s="5"/>
-    </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B133" s="4"/>
-      <c r="C133" s="49"/>
-      <c r="D133" s="43"/>
-      <c r="E133" s="44"/>
-      <c r="F133" s="45"/>
-      <c r="G133" s="43"/>
-      <c r="H133" s="46"/>
-      <c r="I133" s="5"/>
-    </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B134" s="4"/>
-      <c r="C134" s="49"/>
-      <c r="D134" s="43"/>
-      <c r="E134" s="44"/>
-      <c r="F134" s="45"/>
-      <c r="G134" s="43"/>
-      <c r="H134" s="46"/>
-      <c r="I134" s="5"/>
-    </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B135" s="4"/>
-      <c r="C135" s="49"/>
-      <c r="D135" s="43"/>
-      <c r="E135" s="44"/>
-      <c r="F135" s="45"/>
-      <c r="G135" s="43"/>
-      <c r="H135" s="46"/>
-      <c r="I135" s="5"/>
-    </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B136" s="4"/>
-      <c r="C136" s="49"/>
-      <c r="D136" s="43"/>
-      <c r="E136" s="44"/>
-      <c r="F136" s="45"/>
-      <c r="G136" s="43"/>
-      <c r="H136" s="46"/>
-      <c r="I136" s="5"/>
-    </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B137" s="4"/>
-      <c r="C137" s="49"/>
-      <c r="D137" s="43"/>
-      <c r="E137" s="44"/>
-      <c r="F137" s="45"/>
-      <c r="G137" s="43"/>
-      <c r="H137" s="46"/>
-      <c r="I137" s="5"/>
-    </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B138" s="4"/>
-      <c r="C138" s="49"/>
-      <c r="D138" s="43"/>
-      <c r="E138" s="44"/>
-      <c r="F138" s="45"/>
-      <c r="G138" s="43"/>
-      <c r="H138" s="46"/>
-      <c r="I138" s="5"/>
-    </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B139" s="4"/>
-      <c r="C139" s="49"/>
-      <c r="D139" s="43"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="45"/>
-      <c r="G139" s="43"/>
-      <c r="H139" s="46"/>
-      <c r="I139" s="5"/>
-    </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B140" s="4"/>
-      <c r="C140" s="49"/>
-      <c r="D140" s="43"/>
-      <c r="E140" s="44"/>
-      <c r="F140" s="45"/>
-      <c r="G140" s="43"/>
-      <c r="H140" s="46"/>
-      <c r="I140" s="5"/>
-    </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B141" s="4"/>
-      <c r="C141" s="49"/>
-      <c r="D141" s="43"/>
-      <c r="E141" s="44"/>
-      <c r="F141" s="45"/>
-      <c r="G141" s="43"/>
-      <c r="H141" s="46"/>
-      <c r="I141" s="5"/>
-    </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B142" s="4"/>
-      <c r="C142" s="49"/>
-      <c r="D142" s="43"/>
-      <c r="E142" s="44"/>
-      <c r="F142" s="45"/>
-      <c r="G142" s="43"/>
-      <c r="H142" s="46"/>
-      <c r="I142" s="5"/>
-    </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B143" s="4"/>
-      <c r="C143" s="49"/>
-      <c r="D143" s="43"/>
-      <c r="E143" s="44"/>
-      <c r="F143" s="45"/>
-      <c r="G143" s="43"/>
-      <c r="H143" s="46"/>
-      <c r="I143" s="5"/>
-    </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B144" s="4"/>
-      <c r="C144" s="49"/>
-      <c r="D144" s="43"/>
-      <c r="E144" s="44"/>
-      <c r="F144" s="45"/>
-      <c r="G144" s="43"/>
-      <c r="H144" s="46"/>
-      <c r="I144" s="5"/>
-    </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B145" s="4"/>
-      <c r="C145" s="49"/>
-      <c r="D145" s="43"/>
-      <c r="E145" s="44"/>
-      <c r="F145" s="45"/>
-      <c r="G145" s="43"/>
-      <c r="H145" s="46"/>
-      <c r="I145" s="5"/>
-    </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B146" s="4"/>
-      <c r="C146" s="49"/>
-      <c r="D146" s="43"/>
-      <c r="E146" s="44"/>
-      <c r="F146" s="45"/>
-      <c r="G146" s="43"/>
-      <c r="H146" s="46"/>
-      <c r="I146" s="5"/>
-    </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B147" s="8"/>
-      <c r="C147" s="21"/>
-      <c r="D147" s="35"/>
-      <c r="E147" s="28"/>
-      <c r="F147" s="18"/>
-      <c r="G147" s="35"/>
-      <c r="H147" s="19"/>
-      <c r="I147" s="9"/>
-    </row>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="35"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="18"/>
+      <c r="G129" s="35"/>
+      <c r="H129" s="19"/>
+      <c r="I129" s="9"/>
+    </row>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="35">
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="G123:G127"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G52:G56"/>
     <mergeCell ref="C114:C121"/>
     <mergeCell ref="G114:G121"/>
     <mergeCell ref="C58:C66"/>
@@ -3811,8 +3679,8 @@
     <mergeCell ref="G75:G80"/>
     <mergeCell ref="G82:G85"/>
     <mergeCell ref="C75:C80"/>
-    <mergeCell ref="C68:C73"/>
-    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C123:C127"/>
     <mergeCell ref="G87:G93"/>
     <mergeCell ref="G68:G73"/>
     <mergeCell ref="A1:E2"/>
@@ -3827,9 +3695,6 @@
     <mergeCell ref="C40:C50"/>
     <mergeCell ref="G40:G50"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="C52:C56"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Rendu TPI 2019 Diego Sanchez
</commit_message>
<xml_diff>
--- a/Documentation/Journal/JournalDSA.xlsx
+++ b/Documentation/Journal/JournalDSA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="200">
   <si>
     <t>Activités</t>
   </si>
@@ -609,6 +609,21 @@
   </si>
   <si>
     <t>Finalisation et impression de mon projet</t>
+  </si>
+  <si>
+    <t>Impression</t>
+  </si>
+  <si>
+    <t>Graver fichier sur les CD pour le rendu</t>
+  </si>
+  <si>
+    <t>Grave de mes CD pour le rendu</t>
+  </si>
+  <si>
+    <t>Fin de projet</t>
+  </si>
+  <si>
+    <t>06.06.2019, total durée</t>
   </si>
 </sst>
 </file>
@@ -1101,6 +1116,18 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1108,18 +1135,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1573,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M172"/>
+  <dimension ref="A1:M175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1594,31 +1609,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="13"/>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="57"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -1680,7 +1695,7 @@
     </row>
     <row r="9" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="56">
+      <c r="C9" s="60">
         <v>43592</v>
       </c>
       <c r="D9" s="39">
@@ -1692,7 +1707,7 @@
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="59" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="16"/>
@@ -2395,7 +2410,7 @@
       <c r="F52" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="58" t="s">
+      <c r="G52" s="55" t="s">
         <v>97</v>
       </c>
       <c r="H52" s="22"/>
@@ -2413,7 +2428,7 @@
       <c r="F53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G53" s="59"/>
+      <c r="G53" s="56"/>
       <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
@@ -2429,7 +2444,7 @@
       <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="59"/>
+      <c r="G54" s="56"/>
       <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
@@ -2445,7 +2460,7 @@
       <c r="F55" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="59"/>
+      <c r="G55" s="56"/>
       <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
@@ -2461,7 +2476,7 @@
       <c r="F56" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G56" s="60"/>
+      <c r="G56" s="57"/>
       <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
@@ -2887,7 +2902,7 @@
       <c r="F82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G82" s="58" t="s">
+      <c r="G82" s="55" t="s">
         <v>137</v>
       </c>
       <c r="H82" s="22"/>
@@ -2905,7 +2920,7 @@
       <c r="F83" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G83" s="59"/>
+      <c r="G83" s="56"/>
       <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
@@ -2921,7 +2936,7 @@
       <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="59"/>
+      <c r="G84" s="56"/>
       <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
@@ -2937,7 +2952,7 @@
       <c r="F85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G85" s="60"/>
+      <c r="G85" s="57"/>
       <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
@@ -3347,7 +3362,7 @@
       <c r="F110" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="G110" s="58" t="s">
+      <c r="G110" s="55" t="s">
         <v>169</v>
       </c>
       <c r="H110" s="47"/>
@@ -3365,7 +3380,7 @@
       <c r="F111" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="G111" s="59"/>
+      <c r="G111" s="56"/>
       <c r="H111" s="47"/>
       <c r="I111" s="5"/>
     </row>
@@ -3381,7 +3396,7 @@
       <c r="F112" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="G112" s="60"/>
+      <c r="G112" s="57"/>
       <c r="H112" s="47"/>
       <c r="I112" s="5"/>
     </row>
@@ -3646,20 +3661,92 @@
       <c r="H128" s="46"/>
       <c r="I128" s="5"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B129" s="8"/>
-      <c r="C129" s="21"/>
-      <c r="D129" s="35"/>
-      <c r="E129" s="28"/>
-      <c r="F129" s="18"/>
-      <c r="G129" s="35"/>
-      <c r="H129" s="19"/>
-      <c r="I129" s="9"/>
-    </row>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B129" s="4"/>
+      <c r="C129" s="48">
+        <v>43622</v>
+      </c>
+      <c r="D129" s="43">
+        <v>20</v>
+      </c>
+      <c r="E129" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F129" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="G129" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="H129" s="47"/>
+      <c r="I129" s="5"/>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B130" s="4"/>
+      <c r="C130" s="50"/>
+      <c r="D130" s="43">
+        <v>70</v>
+      </c>
+      <c r="E130" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="F130" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="G130" s="53"/>
+      <c r="H130" s="47"/>
+      <c r="I130" s="5"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B131" s="4"/>
+      <c r="C131" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D131" s="43">
+        <f>SUM(D129:D130)</f>
+        <v>90</v>
+      </c>
+      <c r="E131" s="44"/>
+      <c r="F131" s="45"/>
+      <c r="G131" s="43"/>
+      <c r="H131" s="46"/>
+      <c r="I131" s="5"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B132" s="8"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="35"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="18"/>
+      <c r="G132" s="35"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="9"/>
+    </row>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="37">
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G129:G130"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G9:G16"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="C9:C16"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="G22:G30"/>
+    <mergeCell ref="G75:G80"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="C75:C80"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C123:C127"/>
+    <mergeCell ref="G87:G93"/>
+    <mergeCell ref="G68:G73"/>
     <mergeCell ref="C68:C73"/>
     <mergeCell ref="C87:C93"/>
     <mergeCell ref="G123:G127"/>
@@ -3676,25 +3763,6 @@
     <mergeCell ref="C95:C102"/>
     <mergeCell ref="G95:G102"/>
     <mergeCell ref="C82:C85"/>
-    <mergeCell ref="G75:G80"/>
-    <mergeCell ref="G82:G85"/>
-    <mergeCell ref="C75:C80"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C123:C127"/>
-    <mergeCell ref="G87:G93"/>
-    <mergeCell ref="G68:G73"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="G9:G16"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="C9:C16"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="G22:G30"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.47244094488188981" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>